<commit_message>
lists: Use get_field_list_from_json from jsondataferret.utils and make outcomes table working
https://github.com/OpenDataServices/indigo-app/issues/3
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/project-public.xlsx
+++ b/indigo/spreadsheetform_guides/project-public.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
   <si>
     <t xml:space="preserve">Project Name</t>
   </si>
@@ -93,6 +93,18 @@
   </si>
   <si>
     <t xml:space="preserve">Outcome Payments (£)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcomes:title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcomes:definition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not in use yet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcomes:source</t>
   </si>
 </sst>
 </file>
@@ -214,7 +226,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -247,8 +259,12 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -331,7 +347,7 @@
   <dimension ref="A4:C11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -339,7 +355,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.62"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -422,10 +438,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:L17"/>
+  <dimension ref="A3:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+      <selection pane="topLeft" activeCell="M6" activeCellId="0" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -464,6 +480,7 @@
       </c>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
+      <c r="M3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
@@ -502,20 +519,50 @@
       <c r="L4" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M4" s="5" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
+      <c r="A5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8"/>
@@ -529,7 +576,8 @@
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8"/>
@@ -544,6 +592,7 @@
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
+      <c r="M7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8"/>
@@ -558,6 +607,7 @@
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
+      <c r="M8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8"/>
@@ -572,6 +622,7 @@
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
+      <c r="M9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8"/>
@@ -586,6 +637,7 @@
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
+      <c r="M10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8"/>
@@ -600,6 +652,7 @@
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
+      <c r="M11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8"/>
@@ -614,6 +667,7 @@
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
+      <c r="M12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8"/>
@@ -628,6 +682,7 @@
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
+      <c r="M13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8"/>
@@ -642,6 +697,7 @@
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
+      <c r="M14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8"/>
@@ -656,6 +712,7 @@
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
+      <c r="M15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8"/>
@@ -670,6 +727,7 @@
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
+      <c r="M16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8"/>
@@ -684,6 +742,7 @@
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
+      <c r="M17" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
organisations: Add reference in project data, import updates to organisation records, fill data when viewing projects
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/project-public.xlsx
+++ b/indigo/spreadsheetform_guides/project-public.xlsx
@@ -10,6 +10,7 @@
   <sheets>
     <sheet name="General Overview" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Outcomes" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Outcome Fund" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
     <t xml:space="preserve">Project Name</t>
   </si>
@@ -105,6 +106,39 @@
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcomes:source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fund</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_funds:title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_funds:id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_funds:organisation/id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_funds:organisation/name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_funds:organisation/type</t>
   </si>
 </sst>
 </file>
@@ -174,14 +208,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF2E75B6"/>
-        <bgColor rgb="FF0066CC"/>
+        <fgColor rgb="FFE7E6E6"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE7E6E6"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FF2E75B6"/>
+        <bgColor rgb="FF0066CC"/>
       </patternFill>
     </fill>
   </fills>
@@ -226,20 +260,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -247,24 +285,24 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -344,10 +382,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A4:C11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -359,66 +397,69 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+    </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="48.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4"/>
+      <c r="A6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3" t="s">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="3"/>
+      <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -462,286 +503,286 @@
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6" t="s">
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6" t="s">
+      <c r="I3" s="7"/>
+      <c r="J3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="5"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="L5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="M5" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
       <c r="M7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
       <c r="M8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
       <c r="M9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
       <c r="M10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
       <c r="M11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
       <c r="M12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
       <c r="M13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
       <c r="M14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
       <c r="M15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
       <c r="M16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
       <c r="M17" s="9"/>
     </row>
   </sheetData>
@@ -759,4 +800,169 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A4:E18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.47"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
data-model: Remove a space in a JSON path, should not have been there
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/project-public.xlsx
+++ b/indigo/spreadsheetform_guides/project-public.xlsx
@@ -325,19 +325,19 @@
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_funds:id</t>
   </si>
   <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_funds:name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_funds:identifier_scheme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_funds:identifier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_funds:organisation_ids</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_funds:country</t>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_funds:name/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_funds:identifier_scheme/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_funds:identifier/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_funds:organisation_ids/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_funds:country/value</t>
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_funds:source_ids</t>
@@ -557,7 +557,7 @@
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:service_provisions:organisation_role_category/value</t>
   </si>
   <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:service_provisions:intervention /value</t>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:service_provisions:intervention/value</t>
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:service_provisions:planned_service/start_date/value</t>
@@ -1308,8 +1308,8 @@
   </sheetPr>
   <dimension ref="A2:F62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3386,7 +3386,7 @@
   <dimension ref="A2:I33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3454,7 +3454,7 @@
       <c r="G4" s="9"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="87" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
         <v>96</v>
       </c>
@@ -3782,7 +3782,7 @@
   <dimension ref="A2:J32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4640,7 +4640,7 @@
   <dimension ref="A7:J37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5090,7 +5090,7 @@
   <dimension ref="A2:M37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M4" activeCellId="0" sqref="M4"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
data-model: Add min/max/exact fields
https://github.com/INDIGO-Initiative/database-app/issues/5
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/project-public.xlsx
+++ b/indigo/spreadsheetform_guides/project-public.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="345">
   <si>
     <t xml:space="preserve">Indigo Project ID</t>
   </si>
@@ -136,61 +136,91 @@
     <t xml:space="preserve">SPREADSHEETFORM:SINGLE:overall_project_finance/total_investment_commitment/currency/value</t>
   </si>
   <si>
+    <t xml:space="preserve">(min amount)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:overall_project_finance/total_investment_commitment/amount/min/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(exact amount)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:overall_project_finance/total_investment_commitment/amount/exact/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(max amount)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:overall_project_finance/total_investment_commitment/amount/max/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(min in USD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:overall_project_finance/total_investment_commitment/amount_usd/min/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(exact in USD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:overall_project_finance/total_investment_commitment/amount_usd/exact/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(max in USD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:overall_project_finance/total_investment_commitment/amount_usd/max/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum potential outcome payment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:overall_project_finance/maximum_potential_outcome_payment/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum potential loss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:overall_project_finance/maximum_potential_loss/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum potential return type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:overall_project_finance/maximum_potential_return_type/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum potential return</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:overall_project_finance/maximum_potential_return/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuration of the Contracting Parties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:overall_project_finance/configuration_contracting_parties/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Investor repayment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:overall_project_finance/investor_repayment/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total outcome payments made</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:overall_project_finance/total_outcome_payments_made/currency/value</t>
+  </si>
+  <si>
     <t xml:space="preserve">(amount)</t>
   </si>
   <si>
-    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:overall_project_finance/total_investment_commitment/amount/value</t>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:overall_project_finance/total_outcome_payments_made/amount/value</t>
   </si>
   <si>
     <t xml:space="preserve">(amount in USD)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:overall_project_finance/total_investment_commitment/amount_usd/value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maximum potential outcome payment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:overall_project_finance/maximum_potential_outcome_payment/value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maximum potential loss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:overall_project_finance/maximum_potential_loss/value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maximum potential return type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:overall_project_finance/maximum_potential_return_type/value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maximum potential return</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:overall_project_finance/maximum_potential_return/value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Configuration of the Contracting Parties</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:overall_project_finance/configuration_contracting_parties/value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Investor repayment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:overall_project_finance/investor_repayment/value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total outcome payments made</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:overall_project_finance/total_outcome_payments_made/currency/value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:overall_project_finance/total_outcome_payments_made/amount/value</t>
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:SINGLE:overall_project_finance/total_outcome_payments_made/amount_usd/value</t>
@@ -723,6 +753,24 @@
     <t xml:space="preserve">Misc</t>
   </si>
   <si>
+    <t xml:space="preserve">Min Amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exact Amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max Amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min in USD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exact in USD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max in USD</t>
+  </si>
+  <si>
     <t xml:space="preserve">Loss</t>
   </si>
   <si>
@@ -752,10 +800,22 @@
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:investments:investment_commitment/currency/value</t>
   </si>
   <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:investments:investment_commitment/amount/value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:investments:investment_commitment/amount_usd/value</t>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:investments:investment_commitment/amount/min/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:investments:investment_commitment/amount/exact/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:investments:investment_commitment/amount/max/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:investments:investment_commitment/amount_usd/min/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:investments:investment_commitment/amount_usd/exact/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:investments:investment_commitment/amount_usd/max/value</t>
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:investments:maximum_potential_loss/value</t>
@@ -1306,7 +1366,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:F62"/>
+  <dimension ref="A2:F66"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1503,7 +1563,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="58.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
         <v>34</v>
@@ -1512,7 +1572,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="58.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3"/>
       <c r="B28" s="3" t="s">
         <v>36</v>
@@ -1521,43 +1581,43 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="s">
+    <row r="29" customFormat="false" ht="58.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="3"/>
       <c r="C29" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="s">
+    <row r="30" customFormat="false" ht="58.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="3"/>
       <c r="C30" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="s">
+    <row r="31" customFormat="false" ht="58.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="3"/>
       <c r="C31" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="s">
+    <row r="32" customFormat="false" ht="58.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="3"/>
       <c r="C32" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
         <v>46</v>
       </c>
@@ -1566,7 +1626,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
         <v>48</v>
       </c>
@@ -1575,232 +1635,268 @@
         <v>49</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="B35" s="3"/>
       <c r="C35" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3" t="s">
-        <v>34</v>
-      </c>
+    <row r="36" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="3"/>
       <c r="C36" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3" t="s">
-        <v>36</v>
-      </c>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="3"/>
       <c r="C37" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B39" s="3"/>
+        <v>58</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C39" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3" t="s">
-        <v>2</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="5" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E43" s="6"/>
-    </row>
-    <row r="44" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B44" s="3"/>
-      <c r="C44" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B45" s="3"/>
-      <c r="C45" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C45" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>70</v>
+      </c>
+      <c r="E47" s="6"/>
+    </row>
+    <row r="48" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51" s="3"/>
+      <c r="C51" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="B52" s="3"/>
-      <c r="C52" s="3" t="s">
-        <v>2</v>
+      <c r="C52" s="5" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>74</v>
+        <v>9</v>
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
       <c r="B54" s="3"/>
       <c r="C54" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B55" s="3"/>
-      <c r="C55" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="3"/>
+      <c r="A56" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="B56" s="3"/>
-      <c r="C56" s="5"/>
-    </row>
-    <row r="57" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C56" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B57" s="3"/>
       <c r="C57" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
-        <v>9</v>
+        <v>86</v>
       </c>
       <c r="B58" s="3"/>
       <c r="C58" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
       <c r="B59" s="3"/>
       <c r="C59" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="5"/>
+    </row>
+    <row r="61" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B61" s="3"/>
-      <c r="C61" s="3" t="s">
+      <c r="C61" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B62" s="3"/>
+      <c r="C62" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B63" s="3"/>
+      <c r="C63" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="D65" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="4"/>
-      <c r="B62" s="4"/>
-      <c r="C62" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>86</v>
+    <row r="66" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1842,44 +1938,44 @@
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I3" s="6" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I4" s="6" t="s">
-        <v>262</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I5" s="6" t="s">
-        <v>263</v>
+        <v>283</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I6" s="6" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E7" s="6" t="s">
-        <v>265</v>
+        <v>285</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>266</v>
+        <v>286</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E8" s="6" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>269</v>
+        <v>289</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1894,44 +1990,44 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>270</v>
+        <v>290</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>271</v>
+        <v>291</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>273</v>
+        <v>293</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>274</v>
+        <v>294</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>275</v>
+        <v>295</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>28</v>
@@ -1939,40 +2035,40 @@
     </row>
     <row r="11" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>281</v>
+        <v>301</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>282</v>
+        <v>302</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>283</v>
+        <v>303</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>284</v>
+        <v>304</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>285</v>
+        <v>305</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>286</v>
+        <v>306</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>287</v>
+        <v>307</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>288</v>
+        <v>308</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>289</v>
+        <v>309</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>290</v>
+        <v>310</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2410,18 +2506,18 @@
   <sheetData>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="6" t="s">
-        <v>291</v>
+        <v>311</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="6" t="s">
-        <v>292</v>
+        <v>312</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>293</v>
+        <v>313</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2437,47 +2533,47 @@
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="3" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>294</v>
+        <v>314</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>295</v>
+        <v>315</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>296</v>
+        <v>316</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>297</v>
+        <v>317</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>298</v>
+        <v>318</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>299</v>
+        <v>319</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>301</v>
+        <v>321</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="M8" s="3" t="s">
         <v>28</v>
@@ -2494,53 +2590,53 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="9" t="s">
-        <v>302</v>
+        <v>322</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>303</v>
+        <v>323</v>
       </c>
       <c r="L9" s="9"/>
       <c r="M9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
-        <v>304</v>
+        <v>324</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>307</v>
+        <v>327</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>308</v>
+        <v>328</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>309</v>
+        <v>329</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>310</v>
+        <v>330</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>311</v>
+        <v>331</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>312</v>
+        <v>332</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>313</v>
+        <v>333</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>314</v>
+        <v>334</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>315</v>
+        <v>335</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>316</v>
+        <v>336</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2997,17 +3093,17 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>317</v>
+        <v>337</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>28</v>
@@ -3015,13 +3111,13 @@
     </row>
     <row r="4" customFormat="false" ht="100.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>318</v>
+        <v>338</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>319</v>
+        <v>339</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3197,17 +3293,17 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>321</v>
+        <v>341</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>28</v>
@@ -3215,13 +3311,13 @@
     </row>
     <row r="4" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>323</v>
+        <v>343</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>324</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3411,32 +3507,32 @@
       <c r="E2" s="9"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>28</v>
@@ -3448,7 +3544,7 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="9" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="9"/>
@@ -3456,28 +3552,28 @@
     </row>
     <row r="5" customFormat="false" ht="87" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3802,45 +3898,45 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9"/>
       <c r="B2" s="3" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>28</v>
@@ -3848,31 +3944,31 @@
     </row>
     <row r="4" customFormat="false" ht="129.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4224,51 +4320,51 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="0" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4276,7 +4372,7 @@
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -4286,31 +4382,31 @@
     </row>
     <row r="8" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4650,19 +4746,19 @@
   <sheetData>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -4671,63 +4767,63 @@
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9"/>
       <c r="B8" s="3" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5110,27 +5206,27 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="6" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="6" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="6" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="6" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="6" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5139,56 +5235,56 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>28</v>
@@ -5196,40 +5292,40 @@
     </row>
     <row r="9" customFormat="false" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5669,43 +5765,43 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="6" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="6" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="6" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="6" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="6" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="6" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5716,56 +5812,56 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="K9" s="3"/>
       <c r="L9" s="3" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="M10" s="3" t="s">
         <v>28</v>
@@ -5773,43 +5869,43 @@
     </row>
     <row r="11" customFormat="false" ht="143.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6253,10 +6349,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:N46"/>
+  <dimension ref="A3:R46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N14" activeCellId="0" sqref="N14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6266,102 +6362,104 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.04"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.42"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="19.04"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.04"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="20.42"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="6" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="6" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="6" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="6" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="6" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="6" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="6" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="6" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>215</v>
+        <v>224</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>217</v>
+        <v>226</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>219</v>
+        <v>228</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>222</v>
+        <v>230</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>225</v>
+        <v>154</v>
+      </c>
+      <c r="K15" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6369,105 +6467,133 @@
       <c r="B16" s="9"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="3" t="s">
-        <v>227</v>
-      </c>
+      <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
-      <c r="J16" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3" t="s">
-        <v>87</v>
-      </c>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="L16" s="3"/>
       <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-    </row>
-    <row r="17" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N16" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+    </row>
+    <row r="17" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>194</v>
+        <v>239</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>195</v>
+        <v>240</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>230</v>
+        <v>241</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>242</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="J17" s="13" t="s">
-        <v>232</v>
+        <v>243</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>244</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="L17" s="9" t="s">
-        <v>94</v>
+        <v>245</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>246</v>
       </c>
       <c r="M17" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="N17" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="P17" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q17" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="172.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>234</v>
+        <v>250</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>235</v>
+        <v>251</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>236</v>
+        <v>252</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>237</v>
+        <v>253</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>238</v>
+        <v>254</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>239</v>
+        <v>255</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>240</v>
+        <v>256</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>242</v>
+        <v>258</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>243</v>
+        <v>259</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="L18" s="11" t="s">
-        <v>245</v>
+        <v>260</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>261</v>
       </c>
       <c r="M18" s="5" t="s">
-        <v>246</v>
+        <v>262</v>
+      </c>
+      <c r="N18" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="O18" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="P18" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q18" s="5" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6482,8 +6608,12 @@
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
-      <c r="L19" s="11"/>
+      <c r="L19" s="5"/>
       <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
@@ -6497,8 +6627,12 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
-      <c r="L20" s="11"/>
+      <c r="L20" s="5"/>
       <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
@@ -6512,8 +6646,12 @@
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
-      <c r="L21" s="11"/>
+      <c r="L21" s="5"/>
       <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
@@ -6527,8 +6665,12 @@
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="11"/>
+      <c r="L22" s="5"/>
       <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
@@ -6542,8 +6684,12 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
-      <c r="L23" s="11"/>
+      <c r="L23" s="5"/>
       <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10"/>
@@ -6557,8 +6703,12 @@
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
-      <c r="L24" s="11"/>
+      <c r="L24" s="5"/>
       <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
@@ -6572,8 +6722,12 @@
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
-      <c r="L25" s="11"/>
+      <c r="L25" s="5"/>
       <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
@@ -6587,8 +6741,12 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
-      <c r="L26" s="11"/>
+      <c r="L26" s="5"/>
       <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
@@ -6602,8 +6760,12 @@
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
-      <c r="L27" s="11"/>
+      <c r="L27" s="5"/>
       <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
@@ -6617,8 +6779,12 @@
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
-      <c r="L28" s="11"/>
+      <c r="L28" s="5"/>
       <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
@@ -6632,8 +6798,12 @@
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
-      <c r="L29" s="11"/>
+      <c r="L29" s="5"/>
       <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="10"/>
@@ -6647,8 +6817,12 @@
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
-      <c r="L30" s="11"/>
+      <c r="L30" s="5"/>
       <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10"/>
@@ -6662,8 +6836,12 @@
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
-      <c r="L31" s="11"/>
+      <c r="L31" s="5"/>
       <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="10"/>
@@ -6677,8 +6855,12 @@
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
-      <c r="L32" s="11"/>
+      <c r="L32" s="5"/>
       <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="10"/>
@@ -6692,8 +6874,12 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
-      <c r="L33" s="11"/>
+      <c r="L33" s="5"/>
       <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="10"/>
@@ -6707,8 +6893,12 @@
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
-      <c r="L34" s="11"/>
+      <c r="L34" s="5"/>
       <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="10"/>
@@ -6722,8 +6912,12 @@
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
-      <c r="L35" s="11"/>
+      <c r="L35" s="5"/>
       <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="10"/>
@@ -6737,8 +6931,12 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
-      <c r="L36" s="11"/>
+      <c r="L36" s="5"/>
       <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="10"/>
@@ -6752,8 +6950,12 @@
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
-      <c r="L37" s="11"/>
+      <c r="L37" s="5"/>
       <c r="M37" s="5"/>
+      <c r="N37" s="5"/>
+      <c r="O37" s="5"/>
+      <c r="P37" s="11"/>
+      <c r="Q37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="10"/>
@@ -6767,8 +6969,12 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
-      <c r="L38" s="11"/>
+      <c r="L38" s="5"/>
       <c r="M38" s="5"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5"/>
+      <c r="P38" s="11"/>
+      <c r="Q38" s="5"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="10"/>
@@ -6782,8 +6988,12 @@
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
-      <c r="L39" s="11"/>
+      <c r="L39" s="5"/>
       <c r="M39" s="5"/>
+      <c r="N39" s="5"/>
+      <c r="O39" s="5"/>
+      <c r="P39" s="11"/>
+      <c r="Q39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="10"/>
@@ -6797,8 +7007,12 @@
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
-      <c r="L40" s="11"/>
+      <c r="L40" s="5"/>
       <c r="M40" s="5"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="5"/>
+      <c r="P40" s="11"/>
+      <c r="Q40" s="5"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="10"/>
@@ -6812,8 +7026,12 @@
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
-      <c r="L41" s="11"/>
+      <c r="L41" s="5"/>
       <c r="M41" s="5"/>
+      <c r="N41" s="5"/>
+      <c r="O41" s="5"/>
+      <c r="P41" s="11"/>
+      <c r="Q41" s="5"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="10"/>
@@ -6827,8 +7045,12 @@
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
       <c r="K42" s="5"/>
-      <c r="L42" s="11"/>
+      <c r="L42" s="5"/>
       <c r="M42" s="5"/>
+      <c r="N42" s="5"/>
+      <c r="O42" s="5"/>
+      <c r="P42" s="11"/>
+      <c r="Q42" s="5"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="10"/>
@@ -6842,8 +7064,12 @@
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
       <c r="K43" s="5"/>
-      <c r="L43" s="11"/>
+      <c r="L43" s="5"/>
       <c r="M43" s="5"/>
+      <c r="N43" s="5"/>
+      <c r="O43" s="5"/>
+      <c r="P43" s="11"/>
+      <c r="Q43" s="5"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="10"/>
@@ -6857,8 +7083,12 @@
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
       <c r="K44" s="5"/>
-      <c r="L44" s="11"/>
+      <c r="L44" s="5"/>
       <c r="M44" s="5"/>
+      <c r="N44" s="5"/>
+      <c r="O44" s="5"/>
+      <c r="P44" s="11"/>
+      <c r="Q44" s="5"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="10"/>
@@ -6872,8 +7102,12 @@
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
       <c r="K45" s="5"/>
-      <c r="L45" s="11"/>
+      <c r="L45" s="5"/>
       <c r="M45" s="5"/>
+      <c r="N45" s="5"/>
+      <c r="O45" s="5"/>
+      <c r="P45" s="11"/>
+      <c r="Q45" s="5"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="10"/>
@@ -6887,15 +7121,19 @@
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
       <c r="K46" s="5"/>
-      <c r="L46" s="11"/>
+      <c r="L46" s="5"/>
       <c r="M46" s="5"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="5"/>
+      <c r="P46" s="11"/>
+      <c r="Q46" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="L16:N16"/>
+    <mergeCell ref="D16:J16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="P16:R16"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -6931,47 +7169,47 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6" t="s">
-        <v>247</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="6" t="s">
-        <v>248</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="6" t="s">
-        <v>249</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="6" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="6" t="s">
-        <v>251</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="6" t="s">
-        <v>252</v>
+        <v>272</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="6" t="s">
-        <v>253</v>
+        <v>273</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="6" t="s">
-        <v>254</v>
+        <v>274</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="6" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6979,23 +7217,23 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>28</v>
@@ -7003,19 +7241,19 @@
     </row>
     <row r="13" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>257</v>
+        <v>277</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>258</v>
+        <v>278</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>259</v>
+        <v>279</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
data-model: Split fund into a seperate model
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/project-public.xlsx
+++ b/indigo/spreadsheetform_guides/project-public.xlsx
@@ -355,19 +355,19 @@
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_funds:id</t>
   </si>
   <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_funds:name/value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_funds:identifier_scheme/value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_funds:identifier/value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_funds:organisation_ids/value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_funds:country/value</t>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_funds:fund/name/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_funds:fund/identifier_scheme/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_funds:fund/identifier/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_funds:fund/organisation_ids/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_funds:fund/country/value</t>
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_funds:source_ids</t>
@@ -1093,7 +1093,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1127,6 +1127,11 @@
       <name val="DejaVu Sans"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1232,7 +1237,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1274,6 +1279,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1999,31 +2012,31 @@
       <c r="A10" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="15" t="s">
         <v>290</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="15" t="s">
         <v>291</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="15" t="s">
         <v>292</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="15" t="s">
         <v>293</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="15" t="s">
         <v>294</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="15" t="s">
         <v>296</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="15" t="s">
         <v>297</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="J10" s="15" t="s">
         <v>298</v>
       </c>
       <c r="K10" s="9" t="s">
@@ -2064,7 +2077,7 @@
       <c r="J11" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="K11" s="11" t="s">
+      <c r="K11" s="13" t="s">
         <v>309</v>
       </c>
       <c r="L11" s="5" t="s">
@@ -2082,7 +2095,7 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="11"/>
+      <c r="K12" s="13"/>
       <c r="L12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2096,7 +2109,7 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="11"/>
+      <c r="K13" s="13"/>
       <c r="L13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2110,7 +2123,7 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="11"/>
+      <c r="K14" s="13"/>
       <c r="L14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2124,7 +2137,7 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
-      <c r="K15" s="11"/>
+      <c r="K15" s="13"/>
       <c r="L15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2138,7 +2151,7 @@
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
-      <c r="K16" s="11"/>
+      <c r="K16" s="13"/>
       <c r="L16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2152,7 +2165,7 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
-      <c r="K17" s="11"/>
+      <c r="K17" s="13"/>
       <c r="L17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2166,7 +2179,7 @@
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
-      <c r="K18" s="11"/>
+      <c r="K18" s="13"/>
       <c r="L18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2180,7 +2193,7 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
-      <c r="K19" s="11"/>
+      <c r="K19" s="13"/>
       <c r="L19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2194,7 +2207,7 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
-      <c r="K20" s="11"/>
+      <c r="K20" s="13"/>
       <c r="L20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2208,7 +2221,7 @@
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
-      <c r="K21" s="11"/>
+      <c r="K21" s="13"/>
       <c r="L21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2222,7 +2235,7 @@
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
-      <c r="K22" s="11"/>
+      <c r="K22" s="13"/>
       <c r="L22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2236,7 +2249,7 @@
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
-      <c r="K23" s="11"/>
+      <c r="K23" s="13"/>
       <c r="L23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2250,7 +2263,7 @@
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
-      <c r="K24" s="11"/>
+      <c r="K24" s="13"/>
       <c r="L24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2264,7 +2277,7 @@
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
-      <c r="K25" s="11"/>
+      <c r="K25" s="13"/>
       <c r="L25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2278,7 +2291,7 @@
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
-      <c r="K26" s="11"/>
+      <c r="K26" s="13"/>
       <c r="L26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2292,7 +2305,7 @@
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
-      <c r="K27" s="11"/>
+      <c r="K27" s="13"/>
       <c r="L27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2306,7 +2319,7 @@
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
-      <c r="K28" s="11"/>
+      <c r="K28" s="13"/>
       <c r="L28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2320,7 +2333,7 @@
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
-      <c r="K29" s="11"/>
+      <c r="K29" s="13"/>
       <c r="L29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2334,7 +2347,7 @@
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
-      <c r="K30" s="11"/>
+      <c r="K30" s="13"/>
       <c r="L30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2348,7 +2361,7 @@
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
-      <c r="K31" s="11"/>
+      <c r="K31" s="13"/>
       <c r="L31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2362,7 +2375,7 @@
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
-      <c r="K32" s="11"/>
+      <c r="K32" s="13"/>
       <c r="L32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2376,7 +2389,7 @@
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
-      <c r="K33" s="11"/>
+      <c r="K33" s="13"/>
       <c r="L33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2390,7 +2403,7 @@
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
-      <c r="K34" s="11"/>
+      <c r="K34" s="13"/>
       <c r="L34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2404,7 +2417,7 @@
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
-      <c r="K35" s="11"/>
+      <c r="K35" s="13"/>
       <c r="L35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2418,7 +2431,7 @@
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
-      <c r="K36" s="11"/>
+      <c r="K36" s="13"/>
       <c r="L36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2432,7 +2445,7 @@
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
-      <c r="K37" s="11"/>
+      <c r="K37" s="13"/>
       <c r="L37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2446,7 +2459,7 @@
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
-      <c r="K38" s="11"/>
+      <c r="K38" s="13"/>
       <c r="L38" s="5"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2460,7 +2473,7 @@
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
-      <c r="K39" s="11"/>
+      <c r="K39" s="13"/>
       <c r="L39" s="5"/>
     </row>
   </sheetData>
@@ -2557,13 +2570,13 @@
       <c r="F8" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="15" t="s">
         <v>317</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="15" t="s">
         <v>318</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="15" t="s">
         <v>319</v>
       </c>
       <c r="J8" s="9" t="s">
@@ -2599,7 +2612,7 @@
       <c r="M9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="13" t="s">
         <v>324</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -2626,13 +2639,13 @@
       <c r="I10" s="5" t="s">
         <v>332</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="J10" s="13" t="s">
         <v>333</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="K10" s="13" t="s">
         <v>334</v>
       </c>
-      <c r="L10" s="11" t="s">
+      <c r="L10" s="13" t="s">
         <v>335</v>
       </c>
       <c r="M10" s="5" t="s">
@@ -2640,7 +2653,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -2649,13 +2662,13 @@
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
       <c r="M11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -2664,13 +2677,13 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
       <c r="M12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -2679,13 +2692,13 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
       <c r="M13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -2694,13 +2707,13 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
       <c r="M14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -2709,13 +2722,13 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
       <c r="M15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -2724,13 +2737,13 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
       <c r="M16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -2739,13 +2752,13 @@
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
       <c r="M17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -2754,13 +2767,13 @@
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
       <c r="M18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -2769,13 +2782,13 @@
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
       <c r="M19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="11"/>
+      <c r="A20" s="13"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -2784,13 +2797,13 @@
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
       <c r="M20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="11"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -2799,13 +2812,13 @@
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
       <c r="M21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="11"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -2814,13 +2827,13 @@
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
       <c r="M22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="11"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -2829,13 +2842,13 @@
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
       <c r="M23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="11"/>
+      <c r="A24" s="13"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -2844,13 +2857,13 @@
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
       <c r="M24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="11"/>
+      <c r="A25" s="13"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -2859,13 +2872,13 @@
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
       <c r="M25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="11"/>
+      <c r="A26" s="13"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -2874,13 +2887,13 @@
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
       <c r="M26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="11"/>
+      <c r="A27" s="13"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -2889,13 +2902,13 @@
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
       <c r="M27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="11"/>
+      <c r="A28" s="13"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -2904,13 +2917,13 @@
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
       <c r="M28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="11"/>
+      <c r="A29" s="13"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -2919,13 +2932,13 @@
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
-      <c r="L29" s="11"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
       <c r="M29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="11"/>
+      <c r="A30" s="13"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -2934,13 +2947,13 @@
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
       <c r="M30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="11"/>
+      <c r="A31" s="13"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -2949,13 +2962,13 @@
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="11"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
       <c r="M31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="11"/>
+      <c r="A32" s="13"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -2964,13 +2977,13 @@
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-      <c r="L32" s="11"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
       <c r="M32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="11"/>
+      <c r="A33" s="13"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -2979,13 +2992,13 @@
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
       <c r="M33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="11"/>
+      <c r="A34" s="13"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -2994,13 +3007,13 @@
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="11"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
       <c r="M34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="11"/>
+      <c r="A35" s="13"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -3009,13 +3022,13 @@
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="11"/>
-      <c r="L35" s="11"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
       <c r="M35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="11"/>
+      <c r="A36" s="13"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -3024,13 +3037,13 @@
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="11"/>
-      <c r="L36" s="11"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
       <c r="M36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="11"/>
+      <c r="A37" s="13"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -3039,13 +3052,13 @@
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="11"/>
-      <c r="L37" s="11"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
       <c r="M37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="11"/>
+      <c r="A38" s="13"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -3054,9 +3067,9 @@
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="11"/>
-      <c r="L38" s="11"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
       <c r="M38" s="5"/>
     </row>
   </sheetData>
@@ -3113,7 +3126,7 @@
       <c r="A4" s="5" t="s">
         <v>338</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="13" t="s">
         <v>339</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -3122,142 +3135,142 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5"/>
-      <c r="B5" s="11"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5"/>
-      <c r="B6" s="11"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5"/>
-      <c r="B7" s="11"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5"/>
-      <c r="B8" s="11"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5"/>
-      <c r="B9" s="11"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5"/>
-      <c r="B10" s="11"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5"/>
-      <c r="B11" s="11"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5"/>
-      <c r="B12" s="11"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5"/>
-      <c r="B13" s="11"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5"/>
-      <c r="B14" s="11"/>
+      <c r="B14" s="13"/>
       <c r="C14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5"/>
-      <c r="B15" s="11"/>
+      <c r="B15" s="13"/>
       <c r="C15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5"/>
-      <c r="B16" s="11"/>
+      <c r="B16" s="13"/>
       <c r="C16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5"/>
-      <c r="B17" s="11"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5"/>
-      <c r="B18" s="11"/>
+      <c r="B18" s="13"/>
       <c r="C18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5"/>
-      <c r="B19" s="11"/>
+      <c r="B19" s="13"/>
       <c r="C19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5"/>
-      <c r="B20" s="11"/>
+      <c r="B20" s="13"/>
       <c r="C20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5"/>
-      <c r="B21" s="11"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5"/>
-      <c r="B22" s="11"/>
+      <c r="B22" s="13"/>
       <c r="C22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5"/>
-      <c r="B23" s="11"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5"/>
-      <c r="B24" s="11"/>
+      <c r="B24" s="13"/>
       <c r="C24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5"/>
-      <c r="B25" s="11"/>
+      <c r="B25" s="13"/>
       <c r="C25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5"/>
-      <c r="B26" s="11"/>
+      <c r="B26" s="13"/>
       <c r="C26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5"/>
-      <c r="B27" s="11"/>
+      <c r="B27" s="13"/>
       <c r="C27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5"/>
-      <c r="B28" s="11"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5"/>
-      <c r="B29" s="11"/>
+      <c r="B29" s="13"/>
       <c r="C29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5"/>
-      <c r="B30" s="11"/>
+      <c r="B30" s="13"/>
       <c r="C30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5"/>
-      <c r="B31" s="11"/>
+      <c r="B31" s="13"/>
       <c r="C31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5"/>
-      <c r="B32" s="11"/>
+      <c r="B32" s="13"/>
       <c r="C32" s="5"/>
     </row>
   </sheetData>
@@ -3313,7 +3326,7 @@
       <c r="A4" s="5" t="s">
         <v>342</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="13" t="s">
         <v>343</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -3322,142 +3335,142 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5"/>
-      <c r="B5" s="11"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5"/>
-      <c r="B6" s="11"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5"/>
-      <c r="B7" s="11"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5"/>
-      <c r="B8" s="11"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5"/>
-      <c r="B9" s="11"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5"/>
-      <c r="B10" s="11"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5"/>
-      <c r="B11" s="11"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5"/>
-      <c r="B12" s="11"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5"/>
-      <c r="B13" s="11"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5"/>
-      <c r="B14" s="11"/>
+      <c r="B14" s="13"/>
       <c r="C14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5"/>
-      <c r="B15" s="11"/>
+      <c r="B15" s="13"/>
       <c r="C15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5"/>
-      <c r="B16" s="11"/>
+      <c r="B16" s="13"/>
       <c r="C16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5"/>
-      <c r="B17" s="11"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5"/>
-      <c r="B18" s="11"/>
+      <c r="B18" s="13"/>
       <c r="C18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5"/>
-      <c r="B19" s="11"/>
+      <c r="B19" s="13"/>
       <c r="C19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5"/>
-      <c r="B20" s="11"/>
+      <c r="B20" s="13"/>
       <c r="C20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5"/>
-      <c r="B21" s="11"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5"/>
-      <c r="B22" s="11"/>
+      <c r="B22" s="13"/>
       <c r="C22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5"/>
-      <c r="B23" s="11"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5"/>
-      <c r="B24" s="11"/>
+      <c r="B24" s="13"/>
       <c r="C24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5"/>
-      <c r="B25" s="11"/>
+      <c r="B25" s="13"/>
       <c r="C25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5"/>
-      <c r="B26" s="11"/>
+      <c r="B26" s="13"/>
       <c r="C26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5"/>
-      <c r="B27" s="11"/>
+      <c r="B27" s="13"/>
       <c r="C27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5"/>
-      <c r="B28" s="11"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5"/>
-      <c r="B29" s="11"/>
+      <c r="B29" s="13"/>
       <c r="C29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5"/>
-      <c r="B30" s="11"/>
+      <c r="B30" s="13"/>
       <c r="C30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5"/>
-      <c r="B31" s="11"/>
+      <c r="B31" s="13"/>
       <c r="C31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5"/>
-      <c r="B32" s="11"/>
+      <c r="B32" s="13"/>
       <c r="C32" s="5"/>
     </row>
   </sheetData>
@@ -3482,7 +3495,7 @@
   <dimension ref="A2:I33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3550,26 +3563,26 @@
       <c r="G4" s="9"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" customFormat="false" ht="87" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="101.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="13" t="s">
         <v>112</v>
       </c>
       <c r="H5" s="5" t="s">
@@ -3581,9 +3594,9 @@
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="11"/>
+      <c r="E6" s="13"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="11"/>
+      <c r="G6" s="13"/>
       <c r="H6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3591,9 +3604,9 @@
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="11"/>
+      <c r="E7" s="13"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="11"/>
+      <c r="G7" s="13"/>
       <c r="H7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3601,9 +3614,9 @@
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="11"/>
+      <c r="E8" s="13"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="11"/>
+      <c r="G8" s="13"/>
       <c r="H8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3611,9 +3624,9 @@
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
-      <c r="E9" s="11"/>
+      <c r="E9" s="13"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="11"/>
+      <c r="G9" s="13"/>
       <c r="H9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3621,9 +3634,9 @@
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="11"/>
+      <c r="E10" s="13"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="11"/>
+      <c r="G10" s="13"/>
       <c r="H10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3631,9 +3644,9 @@
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="11"/>
+      <c r="E11" s="13"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="11"/>
+      <c r="G11" s="13"/>
       <c r="H11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3641,9 +3654,9 @@
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="11"/>
+      <c r="E12" s="13"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="11"/>
+      <c r="G12" s="13"/>
       <c r="H12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3651,9 +3664,9 @@
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="11"/>
+      <c r="E13" s="13"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="11"/>
+      <c r="G13" s="13"/>
       <c r="H13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3661,9 +3674,9 @@
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="11"/>
+      <c r="E14" s="13"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="11"/>
+      <c r="G14" s="13"/>
       <c r="H14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3671,9 +3684,9 @@
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
-      <c r="E15" s="11"/>
+      <c r="E15" s="13"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="11"/>
+      <c r="G15" s="13"/>
       <c r="H15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3681,9 +3694,9 @@
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="11"/>
+      <c r="E16" s="13"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="11"/>
+      <c r="G16" s="13"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3691,9 +3704,9 @@
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="11"/>
+      <c r="E17" s="13"/>
       <c r="F17" s="5"/>
-      <c r="G17" s="11"/>
+      <c r="G17" s="13"/>
       <c r="H17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3701,9 +3714,9 @@
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="11"/>
+      <c r="E18" s="13"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="11"/>
+      <c r="G18" s="13"/>
       <c r="H18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3711,9 +3724,9 @@
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="11"/>
+      <c r="E19" s="13"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="11"/>
+      <c r="G19" s="13"/>
       <c r="H19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3721,9 +3734,9 @@
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
-      <c r="E20" s="11"/>
+      <c r="E20" s="13"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="11"/>
+      <c r="G20" s="13"/>
       <c r="H20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3731,9 +3744,9 @@
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="11"/>
+      <c r="E21" s="13"/>
       <c r="F21" s="5"/>
-      <c r="G21" s="11"/>
+      <c r="G21" s="13"/>
       <c r="H21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3741,9 +3754,9 @@
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
-      <c r="E22" s="11"/>
+      <c r="E22" s="13"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="11"/>
+      <c r="G22" s="13"/>
       <c r="H22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3751,9 +3764,9 @@
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
-      <c r="E23" s="11"/>
+      <c r="E23" s="13"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="11"/>
+      <c r="G23" s="13"/>
       <c r="H23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3761,9 +3774,9 @@
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="11"/>
+      <c r="E24" s="13"/>
       <c r="F24" s="5"/>
-      <c r="G24" s="11"/>
+      <c r="G24" s="13"/>
       <c r="H24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3771,9 +3784,9 @@
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
-      <c r="E25" s="11"/>
+      <c r="E25" s="13"/>
       <c r="F25" s="5"/>
-      <c r="G25" s="11"/>
+      <c r="G25" s="13"/>
       <c r="H25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3781,9 +3794,9 @@
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
-      <c r="E26" s="11"/>
+      <c r="E26" s="13"/>
       <c r="F26" s="5"/>
-      <c r="G26" s="11"/>
+      <c r="G26" s="13"/>
       <c r="H26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3791,9 +3804,9 @@
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="11"/>
+      <c r="E27" s="13"/>
       <c r="F27" s="5"/>
-      <c r="G27" s="11"/>
+      <c r="G27" s="13"/>
       <c r="H27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3801,9 +3814,9 @@
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
-      <c r="E28" s="11"/>
+      <c r="E28" s="13"/>
       <c r="F28" s="5"/>
-      <c r="G28" s="11"/>
+      <c r="G28" s="13"/>
       <c r="H28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3811,9 +3824,9 @@
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
-      <c r="E29" s="11"/>
+      <c r="E29" s="13"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="11"/>
+      <c r="G29" s="13"/>
       <c r="H29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3821,9 +3834,9 @@
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="11"/>
+      <c r="E30" s="13"/>
       <c r="F30" s="5"/>
-      <c r="G30" s="11"/>
+      <c r="G30" s="13"/>
       <c r="H30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3831,9 +3844,9 @@
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="11"/>
+      <c r="E31" s="13"/>
       <c r="F31" s="5"/>
-      <c r="G31" s="11"/>
+      <c r="G31" s="13"/>
       <c r="H31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3841,9 +3854,9 @@
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="11"/>
+      <c r="E32" s="13"/>
       <c r="F32" s="5"/>
-      <c r="G32" s="11"/>
+      <c r="G32" s="13"/>
       <c r="H32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3851,9 +3864,9 @@
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
-      <c r="E33" s="11"/>
+      <c r="E33" s="13"/>
       <c r="F33" s="5"/>
-      <c r="G33" s="11"/>
+      <c r="G33" s="13"/>
       <c r="H33" s="5"/>
     </row>
   </sheetData>
@@ -3943,7 +3956,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="129.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="13" t="s">
         <v>120</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -3964,7 +3977,7 @@
       <c r="G4" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="13" t="s">
         <v>127</v>
       </c>
       <c r="I4" s="5" t="s">
@@ -3972,311 +3985,311 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="11"/>
+      <c r="H5" s="13"/>
       <c r="I5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="11"/>
+      <c r="H6" s="13"/>
       <c r="I6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="11"/>
+      <c r="H7" s="13"/>
       <c r="I7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="11"/>
+      <c r="H8" s="13"/>
       <c r="I8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="11"/>
+      <c r="H9" s="13"/>
       <c r="I9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="11"/>
+      <c r="H10" s="13"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="11"/>
+      <c r="H11" s="13"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="11"/>
+      <c r="H12" s="13"/>
       <c r="I12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="11"/>
+      <c r="H13" s="13"/>
       <c r="I13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="11"/>
+      <c r="H14" s="13"/>
       <c r="I14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="11"/>
+      <c r="H15" s="13"/>
       <c r="I15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="11"/>
+      <c r="H16" s="13"/>
       <c r="I16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="11"/>
+      <c r="H17" s="13"/>
       <c r="I17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
-      <c r="H18" s="11"/>
+      <c r="H18" s="13"/>
       <c r="I18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="11"/>
+      <c r="H19" s="13"/>
       <c r="I19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="11"/>
+      <c r="A20" s="13"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="11"/>
+      <c r="H20" s="13"/>
       <c r="I20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="11"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
-      <c r="H21" s="11"/>
+      <c r="H21" s="13"/>
       <c r="I21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="11"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
-      <c r="H22" s="11"/>
+      <c r="H22" s="13"/>
       <c r="I22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="11"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="11"/>
+      <c r="H23" s="13"/>
       <c r="I23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="11"/>
+      <c r="A24" s="13"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="11"/>
+      <c r="H24" s="13"/>
       <c r="I24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="11"/>
+      <c r="A25" s="13"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="11"/>
+      <c r="H25" s="13"/>
       <c r="I25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="11"/>
+      <c r="A26" s="13"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
-      <c r="H26" s="11"/>
+      <c r="H26" s="13"/>
       <c r="I26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="11"/>
+      <c r="A27" s="13"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
-      <c r="H27" s="11"/>
+      <c r="H27" s="13"/>
       <c r="I27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="11"/>
+      <c r="A28" s="13"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
-      <c r="H28" s="11"/>
+      <c r="H28" s="13"/>
       <c r="I28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="11"/>
+      <c r="A29" s="13"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
-      <c r="H29" s="11"/>
+      <c r="H29" s="13"/>
       <c r="I29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="11"/>
+      <c r="A30" s="13"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
-      <c r="H30" s="11"/>
+      <c r="H30" s="13"/>
       <c r="I30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="11"/>
+      <c r="A31" s="13"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
-      <c r="H31" s="11"/>
+      <c r="H31" s="13"/>
       <c r="I31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="11"/>
+      <c r="A32" s="13"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
-      <c r="H32" s="11"/>
+      <c r="H32" s="13"/>
       <c r="I32" s="5"/>
     </row>
   </sheetData>
@@ -4381,7 +4394,7 @@
       <c r="I7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="14" t="s">
         <v>140</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -4410,7 +4423,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12"/>
+      <c r="A9" s="14"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -4421,7 +4434,7 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -4432,7 +4445,7 @@
       <c r="I10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -4443,7 +4456,7 @@
       <c r="I11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12"/>
+      <c r="A12" s="14"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -4454,7 +4467,7 @@
       <c r="I12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -4465,7 +4478,7 @@
       <c r="I13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -4476,7 +4489,7 @@
       <c r="I14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -4487,7 +4500,7 @@
       <c r="I15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -4498,7 +4511,7 @@
       <c r="I16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12"/>
+      <c r="A17" s="14"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -4509,7 +4522,7 @@
       <c r="I17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="12"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -4520,7 +4533,7 @@
       <c r="I18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -4531,7 +4544,7 @@
       <c r="I19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="12"/>
+      <c r="A20" s="14"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -4542,7 +4555,7 @@
       <c r="I20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12"/>
+      <c r="A21" s="14"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -4553,7 +4566,7 @@
       <c r="I21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12"/>
+      <c r="A22" s="14"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -4564,7 +4577,7 @@
       <c r="I22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="12"/>
+      <c r="A23" s="14"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -4575,7 +4588,7 @@
       <c r="I23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="12"/>
+      <c r="A24" s="14"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -4586,7 +4599,7 @@
       <c r="I24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="12"/>
+      <c r="A25" s="14"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -4597,7 +4610,7 @@
       <c r="I25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="12"/>
+      <c r="A26" s="14"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -4608,7 +4621,7 @@
       <c r="I26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="12"/>
+      <c r="A27" s="14"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -4619,7 +4632,7 @@
       <c r="I27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="12"/>
+      <c r="A28" s="14"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -4630,7 +4643,7 @@
       <c r="I28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="12"/>
+      <c r="A29" s="14"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -4641,7 +4654,7 @@
       <c r="I29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="12"/>
+      <c r="A30" s="14"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -4652,7 +4665,7 @@
       <c r="I30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="12"/>
+      <c r="A31" s="14"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -4663,7 +4676,7 @@
       <c r="I31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="12"/>
+      <c r="A32" s="14"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -4674,7 +4687,7 @@
       <c r="I32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="12"/>
+      <c r="A33" s="14"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -4685,7 +4698,7 @@
       <c r="I33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="12"/>
+      <c r="A34" s="14"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -4696,7 +4709,7 @@
       <c r="I34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="12"/>
+      <c r="A35" s="14"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -4707,7 +4720,7 @@
       <c r="I35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="12"/>
+      <c r="A36" s="14"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -4795,7 +4808,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="13" t="s">
         <v>157</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -4827,7 +4840,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -4839,7 +4852,7 @@
       <c r="J10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -4851,7 +4864,7 @@
       <c r="J11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -4863,7 +4876,7 @@
       <c r="J12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -4875,7 +4888,7 @@
       <c r="J13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -4887,7 +4900,7 @@
       <c r="J14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -4899,7 +4912,7 @@
       <c r="J15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -4911,7 +4924,7 @@
       <c r="J16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -4923,7 +4936,7 @@
       <c r="J17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -4935,7 +4948,7 @@
       <c r="J18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -4947,7 +4960,7 @@
       <c r="J19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="11"/>
+      <c r="A20" s="13"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -4959,7 +4972,7 @@
       <c r="J20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="11"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -4971,7 +4984,7 @@
       <c r="J21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="11"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -4983,7 +4996,7 @@
       <c r="J22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="11"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -4995,7 +5008,7 @@
       <c r="J23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="11"/>
+      <c r="A24" s="13"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -5007,7 +5020,7 @@
       <c r="J24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="11"/>
+      <c r="A25" s="13"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -5019,7 +5032,7 @@
       <c r="J25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="11"/>
+      <c r="A26" s="13"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -5031,7 +5044,7 @@
       <c r="J26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="11"/>
+      <c r="A27" s="13"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -5043,7 +5056,7 @@
       <c r="J27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="11"/>
+      <c r="A28" s="13"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -5055,7 +5068,7 @@
       <c r="J28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="11"/>
+      <c r="A29" s="13"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -5067,7 +5080,7 @@
       <c r="J29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="11"/>
+      <c r="A30" s="13"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -5079,7 +5092,7 @@
       <c r="J30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="11"/>
+      <c r="A31" s="13"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -5091,7 +5104,7 @@
       <c r="J31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="11"/>
+      <c r="A32" s="13"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -5103,7 +5116,7 @@
       <c r="J32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="11"/>
+      <c r="A33" s="13"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -5115,7 +5128,7 @@
       <c r="J33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="11"/>
+      <c r="A34" s="13"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -5127,7 +5140,7 @@
       <c r="J34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="11"/>
+      <c r="A35" s="13"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -5139,7 +5152,7 @@
       <c r="J35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="11"/>
+      <c r="A36" s="13"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -5151,7 +5164,7 @@
       <c r="J36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="11"/>
+      <c r="A37" s="13"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -5259,7 +5272,7 @@
       <c r="B8" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="15" t="s">
         <v>176</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -5294,7 +5307,7 @@
       <c r="A9" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="13" t="s">
         <v>182</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -5321,7 +5334,7 @@
       <c r="J9" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="K9" s="13" t="s">
         <v>191</v>
       </c>
       <c r="L9" s="5" t="s">
@@ -5330,7 +5343,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -5339,12 +5352,12 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="11"/>
+      <c r="K10" s="13"/>
       <c r="L10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -5353,12 +5366,12 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="11"/>
+      <c r="K11" s="13"/>
       <c r="L11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -5367,12 +5380,12 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="11"/>
+      <c r="K12" s="13"/>
       <c r="L12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -5381,12 +5394,12 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="11"/>
+      <c r="K13" s="13"/>
       <c r="L13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10"/>
-      <c r="B14" s="11"/>
+      <c r="B14" s="13"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -5395,12 +5408,12 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="11"/>
+      <c r="K14" s="13"/>
       <c r="L14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10"/>
-      <c r="B15" s="11"/>
+      <c r="B15" s="13"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -5409,12 +5422,12 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
-      <c r="K15" s="11"/>
+      <c r="K15" s="13"/>
       <c r="L15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10"/>
-      <c r="B16" s="11"/>
+      <c r="B16" s="13"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -5423,12 +5436,12 @@
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
-      <c r="K16" s="11"/>
+      <c r="K16" s="13"/>
       <c r="L16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -5437,12 +5450,12 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
-      <c r="K17" s="11"/>
+      <c r="K17" s="13"/>
       <c r="L17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10"/>
-      <c r="B18" s="11"/>
+      <c r="B18" s="13"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -5451,12 +5464,12 @@
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
-      <c r="K18" s="11"/>
+      <c r="K18" s="13"/>
       <c r="L18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
+      <c r="B19" s="13"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -5465,12 +5478,12 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
-      <c r="K19" s="11"/>
+      <c r="K19" s="13"/>
       <c r="L19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
+      <c r="B20" s="13"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -5479,12 +5492,12 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
-      <c r="K20" s="11"/>
+      <c r="K20" s="13"/>
       <c r="L20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -5493,12 +5506,12 @@
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
-      <c r="K21" s="11"/>
+      <c r="K21" s="13"/>
       <c r="L21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
-      <c r="B22" s="11"/>
+      <c r="B22" s="13"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -5507,12 +5520,12 @@
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
-      <c r="K22" s="11"/>
+      <c r="K22" s="13"/>
       <c r="L22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
-      <c r="B23" s="11"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
@@ -5521,12 +5534,12 @@
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
-      <c r="K23" s="11"/>
+      <c r="K23" s="13"/>
       <c r="L23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10"/>
-      <c r="B24" s="11"/>
+      <c r="B24" s="13"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
@@ -5535,12 +5548,12 @@
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
-      <c r="K24" s="11"/>
+      <c r="K24" s="13"/>
       <c r="L24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
-      <c r="B25" s="11"/>
+      <c r="B25" s="13"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
@@ -5549,12 +5562,12 @@
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
-      <c r="K25" s="11"/>
+      <c r="K25" s="13"/>
       <c r="L25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
-      <c r="B26" s="11"/>
+      <c r="B26" s="13"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
@@ -5563,12 +5576,12 @@
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
-      <c r="K26" s="11"/>
+      <c r="K26" s="13"/>
       <c r="L26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
-      <c r="B27" s="11"/>
+      <c r="B27" s="13"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
@@ -5577,12 +5590,12 @@
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
-      <c r="K27" s="11"/>
+      <c r="K27" s="13"/>
       <c r="L27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
-      <c r="B28" s="11"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
@@ -5591,12 +5604,12 @@
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
-      <c r="K28" s="11"/>
+      <c r="K28" s="13"/>
       <c r="L28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
-      <c r="B29" s="11"/>
+      <c r="B29" s="13"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
@@ -5605,12 +5618,12 @@
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
-      <c r="K29" s="11"/>
+      <c r="K29" s="13"/>
       <c r="L29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="10"/>
-      <c r="B30" s="11"/>
+      <c r="B30" s="13"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
@@ -5619,12 +5632,12 @@
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
-      <c r="K30" s="11"/>
+      <c r="K30" s="13"/>
       <c r="L30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10"/>
-      <c r="B31" s="11"/>
+      <c r="B31" s="13"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
@@ -5633,12 +5646,12 @@
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
-      <c r="K31" s="11"/>
+      <c r="K31" s="13"/>
       <c r="L31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="10"/>
-      <c r="B32" s="11"/>
+      <c r="B32" s="13"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
@@ -5647,12 +5660,12 @@
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
-      <c r="K32" s="11"/>
+      <c r="K32" s="13"/>
       <c r="L32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="10"/>
-      <c r="B33" s="11"/>
+      <c r="B33" s="13"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
@@ -5661,12 +5674,12 @@
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
-      <c r="K33" s="11"/>
+      <c r="K33" s="13"/>
       <c r="L33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="10"/>
-      <c r="B34" s="11"/>
+      <c r="B34" s="13"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
@@ -5675,12 +5688,12 @@
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
-      <c r="K34" s="11"/>
+      <c r="K34" s="13"/>
       <c r="L34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="10"/>
-      <c r="B35" s="11"/>
+      <c r="B35" s="13"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
@@ -5689,12 +5702,12 @@
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
-      <c r="K35" s="11"/>
+      <c r="K35" s="13"/>
       <c r="L35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="10"/>
-      <c r="B36" s="11"/>
+      <c r="B36" s="13"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
@@ -5703,12 +5716,12 @@
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
-      <c r="K36" s="11"/>
+      <c r="K36" s="13"/>
       <c r="L36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="10"/>
-      <c r="B37" s="11"/>
+      <c r="B37" s="13"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
@@ -5717,7 +5730,7 @@
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
-      <c r="K37" s="11"/>
+      <c r="K37" s="13"/>
       <c r="L37" s="5"/>
     </row>
   </sheetData>
@@ -5830,10 +5843,10 @@
       <c r="A10" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="15" t="s">
         <v>199</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -5868,7 +5881,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="143.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="13" t="s">
         <v>206</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -5901,7 +5914,7 @@
       <c r="K11" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="L11" s="11" t="s">
+      <c r="L11" s="13" t="s">
         <v>217</v>
       </c>
       <c r="M11" s="5" t="s">
@@ -5909,7 +5922,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -5920,11 +5933,11 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
-      <c r="L12" s="11"/>
+      <c r="L12" s="13"/>
       <c r="M12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -5935,11 +5948,11 @@
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="11"/>
+      <c r="L13" s="13"/>
       <c r="M13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -5950,11 +5963,11 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
-      <c r="L14" s="11"/>
+      <c r="L14" s="13"/>
       <c r="M14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -5965,11 +5978,11 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
-      <c r="L15" s="11"/>
+      <c r="L15" s="13"/>
       <c r="M15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -5980,11 +5993,11 @@
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
-      <c r="L16" s="11"/>
+      <c r="L16" s="13"/>
       <c r="M16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -5995,11 +6008,11 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
-      <c r="L17" s="11"/>
+      <c r="L17" s="13"/>
       <c r="M17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -6010,11 +6023,11 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
-      <c r="L18" s="11"/>
+      <c r="L18" s="13"/>
       <c r="M18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -6025,11 +6038,11 @@
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
-      <c r="L19" s="11"/>
+      <c r="L19" s="13"/>
       <c r="M19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="11"/>
+      <c r="A20" s="13"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -6040,11 +6053,11 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
-      <c r="L20" s="11"/>
+      <c r="L20" s="13"/>
       <c r="M20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="11"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -6055,11 +6068,11 @@
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
-      <c r="L21" s="11"/>
+      <c r="L21" s="13"/>
       <c r="M21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="11"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -6070,11 +6083,11 @@
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="11"/>
+      <c r="L22" s="13"/>
       <c r="M22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="11"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -6085,11 +6098,11 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
-      <c r="L23" s="11"/>
+      <c r="L23" s="13"/>
       <c r="M23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="11"/>
+      <c r="A24" s="13"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -6100,11 +6113,11 @@
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
-      <c r="L24" s="11"/>
+      <c r="L24" s="13"/>
       <c r="M24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="11"/>
+      <c r="A25" s="13"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -6115,11 +6128,11 @@
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
-      <c r="L25" s="11"/>
+      <c r="L25" s="13"/>
       <c r="M25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="11"/>
+      <c r="A26" s="13"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -6130,11 +6143,11 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
-      <c r="L26" s="11"/>
+      <c r="L26" s="13"/>
       <c r="M26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="11"/>
+      <c r="A27" s="13"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -6145,11 +6158,11 @@
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
-      <c r="L27" s="11"/>
+      <c r="L27" s="13"/>
       <c r="M27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="11"/>
+      <c r="A28" s="13"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -6160,11 +6173,11 @@
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
-      <c r="L28" s="11"/>
+      <c r="L28" s="13"/>
       <c r="M28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="11"/>
+      <c r="A29" s="13"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -6175,11 +6188,11 @@
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
-      <c r="L29" s="11"/>
+      <c r="L29" s="13"/>
       <c r="M29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="11"/>
+      <c r="A30" s="13"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -6190,11 +6203,11 @@
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
-      <c r="L30" s="11"/>
+      <c r="L30" s="13"/>
       <c r="M30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="11"/>
+      <c r="A31" s="13"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -6205,11 +6218,11 @@
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
-      <c r="L31" s="11"/>
+      <c r="L31" s="13"/>
       <c r="M31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="11"/>
+      <c r="A32" s="13"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -6220,11 +6233,11 @@
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
-      <c r="L32" s="11"/>
+      <c r="L32" s="13"/>
       <c r="M32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="11"/>
+      <c r="A33" s="13"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -6235,11 +6248,11 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
-      <c r="L33" s="11"/>
+      <c r="L33" s="13"/>
       <c r="M33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="11"/>
+      <c r="A34" s="13"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -6250,11 +6263,11 @@
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
-      <c r="L34" s="11"/>
+      <c r="L34" s="13"/>
       <c r="M34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="11"/>
+      <c r="A35" s="13"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -6265,11 +6278,11 @@
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
-      <c r="L35" s="11"/>
+      <c r="L35" s="13"/>
       <c r="M35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="11"/>
+      <c r="A36" s="13"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -6280,11 +6293,11 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
-      <c r="L36" s="11"/>
+      <c r="L36" s="13"/>
       <c r="M36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="11"/>
+      <c r="A37" s="13"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -6295,11 +6308,11 @@
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
-      <c r="L37" s="11"/>
+      <c r="L37" s="13"/>
       <c r="M37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="11"/>
+      <c r="A38" s="13"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -6310,11 +6323,11 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
-      <c r="L38" s="11"/>
+      <c r="L38" s="13"/>
       <c r="M38" s="5"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="11"/>
+      <c r="A39" s="13"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -6325,7 +6338,7 @@
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
-      <c r="L39" s="11"/>
+      <c r="L39" s="13"/>
       <c r="M39" s="5"/>
     </row>
   </sheetData>
@@ -6497,7 +6510,7 @@
       <c r="B17" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="15" t="s">
         <v>176</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -6524,13 +6537,13 @@
       <c r="K17" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="L17" s="13" t="s">
+      <c r="L17" s="15" t="s">
         <v>246</v>
       </c>
       <c r="M17" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="N17" s="13" t="s">
+      <c r="N17" s="15" t="s">
         <v>248</v>
       </c>
       <c r="O17" s="3" t="s">
@@ -6547,7 +6560,7 @@
       <c r="A18" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="13" t="s">
         <v>251</v>
       </c>
       <c r="C18" s="5" t="s">
@@ -6589,7 +6602,7 @@
       <c r="O18" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="P18" s="11" t="s">
+      <c r="P18" s="13" t="s">
         <v>265</v>
       </c>
       <c r="Q18" s="5" t="s">
@@ -6598,7 +6611,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
+      <c r="B19" s="13"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -6612,12 +6625,12 @@
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
-      <c r="P19" s="11"/>
+      <c r="P19" s="13"/>
       <c r="Q19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
+      <c r="B20" s="13"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -6631,12 +6644,12 @@
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
-      <c r="P20" s="11"/>
+      <c r="P20" s="13"/>
       <c r="Q20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -6650,12 +6663,12 @@
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
-      <c r="P21" s="11"/>
+      <c r="P21" s="13"/>
       <c r="Q21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
-      <c r="B22" s="11"/>
+      <c r="B22" s="13"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -6669,12 +6682,12 @@
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
-      <c r="P22" s="11"/>
+      <c r="P22" s="13"/>
       <c r="Q22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
-      <c r="B23" s="11"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
@@ -6688,12 +6701,12 @@
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
-      <c r="P23" s="11"/>
+      <c r="P23" s="13"/>
       <c r="Q23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10"/>
-      <c r="B24" s="11"/>
+      <c r="B24" s="13"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
@@ -6707,12 +6720,12 @@
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
-      <c r="P24" s="11"/>
+      <c r="P24" s="13"/>
       <c r="Q24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
-      <c r="B25" s="11"/>
+      <c r="B25" s="13"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
@@ -6726,12 +6739,12 @@
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
-      <c r="P25" s="11"/>
+      <c r="P25" s="13"/>
       <c r="Q25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
-      <c r="B26" s="11"/>
+      <c r="B26" s="13"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
@@ -6745,12 +6758,12 @@
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
-      <c r="P26" s="11"/>
+      <c r="P26" s="13"/>
       <c r="Q26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
-      <c r="B27" s="11"/>
+      <c r="B27" s="13"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
@@ -6764,12 +6777,12 @@
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
-      <c r="P27" s="11"/>
+      <c r="P27" s="13"/>
       <c r="Q27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
-      <c r="B28" s="11"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
@@ -6783,12 +6796,12 @@
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
-      <c r="P28" s="11"/>
+      <c r="P28" s="13"/>
       <c r="Q28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
-      <c r="B29" s="11"/>
+      <c r="B29" s="13"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
@@ -6802,12 +6815,12 @@
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
-      <c r="P29" s="11"/>
+      <c r="P29" s="13"/>
       <c r="Q29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="10"/>
-      <c r="B30" s="11"/>
+      <c r="B30" s="13"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
@@ -6821,12 +6834,12 @@
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
-      <c r="P30" s="11"/>
+      <c r="P30" s="13"/>
       <c r="Q30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10"/>
-      <c r="B31" s="11"/>
+      <c r="B31" s="13"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
@@ -6840,12 +6853,12 @@
       <c r="M31" s="5"/>
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
-      <c r="P31" s="11"/>
+      <c r="P31" s="13"/>
       <c r="Q31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="10"/>
-      <c r="B32" s="11"/>
+      <c r="B32" s="13"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
@@ -6859,12 +6872,12 @@
       <c r="M32" s="5"/>
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
-      <c r="P32" s="11"/>
+      <c r="P32" s="13"/>
       <c r="Q32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="10"/>
-      <c r="B33" s="11"/>
+      <c r="B33" s="13"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
@@ -6878,12 +6891,12 @@
       <c r="M33" s="5"/>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
-      <c r="P33" s="11"/>
+      <c r="P33" s="13"/>
       <c r="Q33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="10"/>
-      <c r="B34" s="11"/>
+      <c r="B34" s="13"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
@@ -6897,12 +6910,12 @@
       <c r="M34" s="5"/>
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
-      <c r="P34" s="11"/>
+      <c r="P34" s="13"/>
       <c r="Q34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="10"/>
-      <c r="B35" s="11"/>
+      <c r="B35" s="13"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
@@ -6916,12 +6929,12 @@
       <c r="M35" s="5"/>
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
-      <c r="P35" s="11"/>
+      <c r="P35" s="13"/>
       <c r="Q35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="10"/>
-      <c r="B36" s="11"/>
+      <c r="B36" s="13"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
@@ -6935,12 +6948,12 @@
       <c r="M36" s="5"/>
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
-      <c r="P36" s="11"/>
+      <c r="P36" s="13"/>
       <c r="Q36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="10"/>
-      <c r="B37" s="11"/>
+      <c r="B37" s="13"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
@@ -6954,12 +6967,12 @@
       <c r="M37" s="5"/>
       <c r="N37" s="5"/>
       <c r="O37" s="5"/>
-      <c r="P37" s="11"/>
+      <c r="P37" s="13"/>
       <c r="Q37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="10"/>
-      <c r="B38" s="11"/>
+      <c r="B38" s="13"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
@@ -6973,12 +6986,12 @@
       <c r="M38" s="5"/>
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
-      <c r="P38" s="11"/>
+      <c r="P38" s="13"/>
       <c r="Q38" s="5"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="10"/>
-      <c r="B39" s="11"/>
+      <c r="B39" s="13"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
@@ -6992,12 +7005,12 @@
       <c r="M39" s="5"/>
       <c r="N39" s="5"/>
       <c r="O39" s="5"/>
-      <c r="P39" s="11"/>
+      <c r="P39" s="13"/>
       <c r="Q39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="10"/>
-      <c r="B40" s="11"/>
+      <c r="B40" s="13"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
@@ -7011,12 +7024,12 @@
       <c r="M40" s="5"/>
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
-      <c r="P40" s="11"/>
+      <c r="P40" s="13"/>
       <c r="Q40" s="5"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="10"/>
-      <c r="B41" s="11"/>
+      <c r="B41" s="13"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
@@ -7030,12 +7043,12 @@
       <c r="M41" s="5"/>
       <c r="N41" s="5"/>
       <c r="O41" s="5"/>
-      <c r="P41" s="11"/>
+      <c r="P41" s="13"/>
       <c r="Q41" s="5"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="10"/>
-      <c r="B42" s="11"/>
+      <c r="B42" s="13"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
@@ -7049,12 +7062,12 @@
       <c r="M42" s="5"/>
       <c r="N42" s="5"/>
       <c r="O42" s="5"/>
-      <c r="P42" s="11"/>
+      <c r="P42" s="13"/>
       <c r="Q42" s="5"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="10"/>
-      <c r="B43" s="11"/>
+      <c r="B43" s="13"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
@@ -7068,12 +7081,12 @@
       <c r="M43" s="5"/>
       <c r="N43" s="5"/>
       <c r="O43" s="5"/>
-      <c r="P43" s="11"/>
+      <c r="P43" s="13"/>
       <c r="Q43" s="5"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="10"/>
-      <c r="B44" s="11"/>
+      <c r="B44" s="13"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
@@ -7087,12 +7100,12 @@
       <c r="M44" s="5"/>
       <c r="N44" s="5"/>
       <c r="O44" s="5"/>
-      <c r="P44" s="11"/>
+      <c r="P44" s="13"/>
       <c r="Q44" s="5"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="10"/>
-      <c r="B45" s="11"/>
+      <c r="B45" s="13"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
@@ -7106,12 +7119,12 @@
       <c r="M45" s="5"/>
       <c r="N45" s="5"/>
       <c r="O45" s="5"/>
-      <c r="P45" s="11"/>
+      <c r="P45" s="13"/>
       <c r="Q45" s="5"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="10"/>
-      <c r="B46" s="11"/>
+      <c r="B46" s="13"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
@@ -7125,7 +7138,7 @@
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
       <c r="O46" s="5"/>
-      <c r="P46" s="11"/>
+      <c r="P46" s="13"/>
       <c r="Q46" s="5"/>
     </row>
   </sheetData>
@@ -7226,10 +7239,10 @@
       <c r="A12" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="15" t="s">
         <v>275</v>
       </c>
       <c r="D12" s="9" t="s">
@@ -7240,7 +7253,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="13" t="s">
         <v>276</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -7249,7 +7262,7 @@
       <c r="C13" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="13" t="s">
         <v>279</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -7257,199 +7270,199 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="11"/>
+      <c r="D14" s="13"/>
       <c r="E14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="11"/>
+      <c r="D15" s="13"/>
       <c r="E15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="11"/>
+      <c r="D16" s="13"/>
       <c r="E16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
-      <c r="D17" s="11"/>
+      <c r="D17" s="13"/>
       <c r="E17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
-      <c r="D18" s="11"/>
+      <c r="D18" s="13"/>
       <c r="E18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="11"/>
+      <c r="D19" s="13"/>
       <c r="E19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="11"/>
+      <c r="A20" s="13"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
-      <c r="D20" s="11"/>
+      <c r="D20" s="13"/>
       <c r="E20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="11"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
-      <c r="D21" s="11"/>
+      <c r="D21" s="13"/>
       <c r="E21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="11"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
-      <c r="D22" s="11"/>
+      <c r="D22" s="13"/>
       <c r="E22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="11"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
-      <c r="D23" s="11"/>
+      <c r="D23" s="13"/>
       <c r="E23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="11"/>
+      <c r="A24" s="13"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
-      <c r="D24" s="11"/>
+      <c r="D24" s="13"/>
       <c r="E24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="11"/>
+      <c r="A25" s="13"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
-      <c r="D25" s="11"/>
+      <c r="D25" s="13"/>
       <c r="E25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="11"/>
+      <c r="A26" s="13"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
-      <c r="D26" s="11"/>
+      <c r="D26" s="13"/>
       <c r="E26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="11"/>
+      <c r="A27" s="13"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
-      <c r="D27" s="11"/>
+      <c r="D27" s="13"/>
       <c r="E27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="11"/>
+      <c r="A28" s="13"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
-      <c r="D28" s="11"/>
+      <c r="D28" s="13"/>
       <c r="E28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="11"/>
+      <c r="A29" s="13"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
-      <c r="D29" s="11"/>
+      <c r="D29" s="13"/>
       <c r="E29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="11"/>
+      <c r="A30" s="13"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
-      <c r="D30" s="11"/>
+      <c r="D30" s="13"/>
       <c r="E30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="11"/>
+      <c r="A31" s="13"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
-      <c r="D31" s="11"/>
+      <c r="D31" s="13"/>
       <c r="E31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="11"/>
+      <c r="A32" s="13"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
-      <c r="D32" s="11"/>
+      <c r="D32" s="13"/>
       <c r="E32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="11"/>
+      <c r="A33" s="13"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
-      <c r="D33" s="11"/>
+      <c r="D33" s="13"/>
       <c r="E33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="11"/>
+      <c r="A34" s="13"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
-      <c r="D34" s="11"/>
+      <c r="D34" s="13"/>
       <c r="E34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="11"/>
+      <c r="A35" s="13"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
-      <c r="D35" s="11"/>
+      <c r="D35" s="13"/>
       <c r="E35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="11"/>
+      <c r="A36" s="13"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
-      <c r="D36" s="11"/>
+      <c r="D36" s="13"/>
       <c r="E36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="11"/>
+      <c r="A37" s="13"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="11"/>
+      <c r="D37" s="13"/>
       <c r="E37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="11"/>
+      <c r="A38" s="13"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="11"/>
+      <c r="D38" s="13"/>
       <c r="E38" s="5"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="11"/>
+      <c r="A39" s="13"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
-      <c r="D39" s="11"/>
+      <c r="D39" s="13"/>
       <c r="E39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="11"/>
+      <c r="A40" s="13"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
-      <c r="D40" s="11"/>
+      <c r="D40" s="13"/>
       <c r="E40" s="5"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="11"/>
+      <c r="A41" s="13"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
-      <c r="D41" s="11"/>
+      <c r="D41" s="13"/>
       <c r="E41" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data-model: Project spreadsheets; remove space in key path
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/project-public.xlsx
+++ b/indigo/spreadsheetform_guides/project-public.xlsx
@@ -972,7 +972,7 @@
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_metrics:outcome_validation_method/value</t>
   </si>
   <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_metrics:data_source_for _outcome_validation/value</t>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_metrics:data_source_for_outcome_validation/value</t>
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_metrics:source_ids</t>
@@ -1093,7 +1093,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1127,11 +1127,6 @@
       <name val="DejaVu Sans"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="DejaVu Sans"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1237,7 +1232,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1279,14 +1274,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1930,8 +1917,8 @@
   </sheetPr>
   <dimension ref="A3:M39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M6" activeCellId="0" sqref="M6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2012,31 +1999,31 @@
       <c r="A10" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="13" t="s">
         <v>290</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="13" t="s">
         <v>292</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="13" t="s">
         <v>293</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="13" t="s">
         <v>294</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="H10" s="15" t="s">
+      <c r="H10" s="13" t="s">
         <v>296</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="I10" s="13" t="s">
         <v>297</v>
       </c>
-      <c r="J10" s="15" t="s">
+      <c r="J10" s="13" t="s">
         <v>298</v>
       </c>
       <c r="K10" s="9" t="s">
@@ -2077,7 +2064,7 @@
       <c r="J11" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="K11" s="13" t="s">
+      <c r="K11" s="11" t="s">
         <v>309</v>
       </c>
       <c r="L11" s="5" t="s">
@@ -2095,7 +2082,7 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="13"/>
+      <c r="K12" s="11"/>
       <c r="L12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2109,7 +2096,7 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="13"/>
+      <c r="K13" s="11"/>
       <c r="L13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2123,7 +2110,7 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="13"/>
+      <c r="K14" s="11"/>
       <c r="L14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2137,7 +2124,7 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
-      <c r="K15" s="13"/>
+      <c r="K15" s="11"/>
       <c r="L15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2151,7 +2138,7 @@
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
-      <c r="K16" s="13"/>
+      <c r="K16" s="11"/>
       <c r="L16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2165,7 +2152,7 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
-      <c r="K17" s="13"/>
+      <c r="K17" s="11"/>
       <c r="L17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2179,7 +2166,7 @@
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
-      <c r="K18" s="13"/>
+      <c r="K18" s="11"/>
       <c r="L18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2193,7 +2180,7 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
-      <c r="K19" s="13"/>
+      <c r="K19" s="11"/>
       <c r="L19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2207,7 +2194,7 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
-      <c r="K20" s="13"/>
+      <c r="K20" s="11"/>
       <c r="L20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2221,7 +2208,7 @@
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
-      <c r="K21" s="13"/>
+      <c r="K21" s="11"/>
       <c r="L21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2235,7 +2222,7 @@
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
-      <c r="K22" s="13"/>
+      <c r="K22" s="11"/>
       <c r="L22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2249,7 +2236,7 @@
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
-      <c r="K23" s="13"/>
+      <c r="K23" s="11"/>
       <c r="L23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2263,7 +2250,7 @@
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
-      <c r="K24" s="13"/>
+      <c r="K24" s="11"/>
       <c r="L24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2277,7 +2264,7 @@
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
-      <c r="K25" s="13"/>
+      <c r="K25" s="11"/>
       <c r="L25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2291,7 +2278,7 @@
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
-      <c r="K26" s="13"/>
+      <c r="K26" s="11"/>
       <c r="L26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2305,7 +2292,7 @@
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
-      <c r="K27" s="13"/>
+      <c r="K27" s="11"/>
       <c r="L27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2319,7 +2306,7 @@
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
-      <c r="K28" s="13"/>
+      <c r="K28" s="11"/>
       <c r="L28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2333,7 +2320,7 @@
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
-      <c r="K29" s="13"/>
+      <c r="K29" s="11"/>
       <c r="L29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2347,7 +2334,7 @@
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
-      <c r="K30" s="13"/>
+      <c r="K30" s="11"/>
       <c r="L30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2361,7 +2348,7 @@
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
-      <c r="K31" s="13"/>
+      <c r="K31" s="11"/>
       <c r="L31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2375,7 +2362,7 @@
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
-      <c r="K32" s="13"/>
+      <c r="K32" s="11"/>
       <c r="L32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2389,7 +2376,7 @@
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
-      <c r="K33" s="13"/>
+      <c r="K33" s="11"/>
       <c r="L33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2403,7 +2390,7 @@
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
-      <c r="K34" s="13"/>
+      <c r="K34" s="11"/>
       <c r="L34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2417,7 +2404,7 @@
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
-      <c r="K35" s="13"/>
+      <c r="K35" s="11"/>
       <c r="L35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2431,7 +2418,7 @@
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
-      <c r="K36" s="13"/>
+      <c r="K36" s="11"/>
       <c r="L36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2445,7 +2432,7 @@
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
-      <c r="K37" s="13"/>
+      <c r="K37" s="11"/>
       <c r="L37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2459,7 +2446,7 @@
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
-      <c r="K38" s="13"/>
+      <c r="K38" s="11"/>
       <c r="L38" s="5"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2473,7 +2460,7 @@
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
-      <c r="K39" s="13"/>
+      <c r="K39" s="11"/>
       <c r="L39" s="5"/>
     </row>
   </sheetData>
@@ -2570,13 +2557,13 @@
       <c r="F8" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="13" t="s">
         <v>317</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="13" t="s">
         <v>318</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="I8" s="13" t="s">
         <v>319</v>
       </c>
       <c r="J8" s="9" t="s">
@@ -2612,7 +2599,7 @@
       <c r="M9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="11" t="s">
         <v>324</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -2639,13 +2626,13 @@
       <c r="I10" s="5" t="s">
         <v>332</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="J10" s="11" t="s">
         <v>333</v>
       </c>
-      <c r="K10" s="13" t="s">
+      <c r="K10" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="L10" s="13" t="s">
+      <c r="L10" s="11" t="s">
         <v>335</v>
       </c>
       <c r="M10" s="5" t="s">
@@ -2653,7 +2640,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -2662,13 +2649,13 @@
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
       <c r="M11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -2677,13 +2664,13 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
       <c r="M12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -2692,13 +2679,13 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
       <c r="M13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -2707,13 +2694,13 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
       <c r="M14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -2722,13 +2709,13 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
       <c r="M15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -2737,13 +2724,13 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
       <c r="M16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -2752,13 +2739,13 @@
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
       <c r="M17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -2767,13 +2754,13 @@
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
       <c r="M18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -2782,13 +2769,13 @@
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
       <c r="M19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -2797,13 +2784,13 @@
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
       <c r="M20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="13"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -2812,13 +2799,13 @@
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
       <c r="M21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="13"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -2827,13 +2814,13 @@
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
       <c r="M22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="13"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -2842,13 +2829,13 @@
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
       <c r="M23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="13"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -2857,13 +2844,13 @@
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
       <c r="M24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="13"/>
+      <c r="A25" s="11"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -2872,13 +2859,13 @@
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
       <c r="M25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="13"/>
+      <c r="A26" s="11"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -2887,13 +2874,13 @@
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
       <c r="M26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="13"/>
+      <c r="A27" s="11"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -2902,13 +2889,13 @@
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
       <c r="M27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="13"/>
+      <c r="A28" s="11"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -2917,13 +2904,13 @@
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
       <c r="M28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="13"/>
+      <c r="A29" s="11"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -2932,13 +2919,13 @@
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
       <c r="M29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="13"/>
+      <c r="A30" s="11"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -2947,13 +2934,13 @@
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
       <c r="M30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="13"/>
+      <c r="A31" s="11"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -2962,13 +2949,13 @@
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
       <c r="M31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="13"/>
+      <c r="A32" s="11"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -2977,13 +2964,13 @@
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
       <c r="M32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="13"/>
+      <c r="A33" s="11"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -2992,13 +2979,13 @@
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
       <c r="M33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="13"/>
+      <c r="A34" s="11"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -3007,13 +2994,13 @@
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="13"/>
-      <c r="L34" s="13"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
       <c r="M34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="13"/>
+      <c r="A35" s="11"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -3022,13 +3009,13 @@
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11"/>
       <c r="M35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="13"/>
+      <c r="A36" s="11"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -3037,13 +3024,13 @@
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
       <c r="M36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="13"/>
+      <c r="A37" s="11"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -3052,13 +3039,13 @@
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11"/>
       <c r="M37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="13"/>
+      <c r="A38" s="11"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -3067,9 +3054,9 @@
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
-      <c r="J38" s="13"/>
-      <c r="K38" s="13"/>
-      <c r="L38" s="13"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="11"/>
       <c r="M38" s="5"/>
     </row>
   </sheetData>
@@ -3126,7 +3113,7 @@
       <c r="A4" s="5" t="s">
         <v>338</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>339</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -3135,142 +3122,142 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5"/>
-      <c r="B5" s="13"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5"/>
-      <c r="B6" s="13"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5"/>
-      <c r="B7" s="13"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5"/>
-      <c r="B8" s="13"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5"/>
-      <c r="B9" s="13"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5"/>
-      <c r="B10" s="13"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5"/>
-      <c r="B11" s="13"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5"/>
-      <c r="B12" s="13"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5"/>
-      <c r="B13" s="13"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5"/>
-      <c r="B14" s="13"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5"/>
-      <c r="B15" s="13"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5"/>
-      <c r="B16" s="13"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5"/>
-      <c r="B17" s="13"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5"/>
-      <c r="B18" s="13"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5"/>
-      <c r="B19" s="13"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5"/>
-      <c r="B20" s="13"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5"/>
-      <c r="B21" s="13"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5"/>
-      <c r="B22" s="13"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5"/>
-      <c r="B23" s="13"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5"/>
-      <c r="B24" s="13"/>
+      <c r="B24" s="11"/>
       <c r="C24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5"/>
-      <c r="B25" s="13"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5"/>
-      <c r="B26" s="13"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5"/>
-      <c r="B27" s="13"/>
+      <c r="B27" s="11"/>
       <c r="C27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5"/>
-      <c r="B28" s="13"/>
+      <c r="B28" s="11"/>
       <c r="C28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5"/>
-      <c r="B29" s="13"/>
+      <c r="B29" s="11"/>
       <c r="C29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5"/>
-      <c r="B30" s="13"/>
+      <c r="B30" s="11"/>
       <c r="C30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5"/>
-      <c r="B31" s="13"/>
+      <c r="B31" s="11"/>
       <c r="C31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5"/>
-      <c r="B32" s="13"/>
+      <c r="B32" s="11"/>
       <c r="C32" s="5"/>
     </row>
   </sheetData>
@@ -3326,7 +3313,7 @@
       <c r="A4" s="5" t="s">
         <v>342</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>343</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -3335,142 +3322,142 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5"/>
-      <c r="B5" s="13"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5"/>
-      <c r="B6" s="13"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5"/>
-      <c r="B7" s="13"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5"/>
-      <c r="B8" s="13"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5"/>
-      <c r="B9" s="13"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5"/>
-      <c r="B10" s="13"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5"/>
-      <c r="B11" s="13"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5"/>
-      <c r="B12" s="13"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5"/>
-      <c r="B13" s="13"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5"/>
-      <c r="B14" s="13"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5"/>
-      <c r="B15" s="13"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5"/>
-      <c r="B16" s="13"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5"/>
-      <c r="B17" s="13"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5"/>
-      <c r="B18" s="13"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5"/>
-      <c r="B19" s="13"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5"/>
-      <c r="B20" s="13"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5"/>
-      <c r="B21" s="13"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5"/>
-      <c r="B22" s="13"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5"/>
-      <c r="B23" s="13"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5"/>
-      <c r="B24" s="13"/>
+      <c r="B24" s="11"/>
       <c r="C24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5"/>
-      <c r="B25" s="13"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5"/>
-      <c r="B26" s="13"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5"/>
-      <c r="B27" s="13"/>
+      <c r="B27" s="11"/>
       <c r="C27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5"/>
-      <c r="B28" s="13"/>
+      <c r="B28" s="11"/>
       <c r="C28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5"/>
-      <c r="B29" s="13"/>
+      <c r="B29" s="11"/>
       <c r="C29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5"/>
-      <c r="B30" s="13"/>
+      <c r="B30" s="11"/>
       <c r="C30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5"/>
-      <c r="B31" s="13"/>
+      <c r="B31" s="11"/>
       <c r="C31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5"/>
-      <c r="B32" s="13"/>
+      <c r="B32" s="11"/>
       <c r="C32" s="5"/>
     </row>
   </sheetData>
@@ -3567,22 +3554,22 @@
       <c r="A5" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="11" t="s">
         <v>112</v>
       </c>
       <c r="H5" s="5" t="s">
@@ -3594,9 +3581,9 @@
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="13"/>
+      <c r="E6" s="11"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="13"/>
+      <c r="G6" s="11"/>
       <c r="H6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3604,9 +3591,9 @@
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="13"/>
+      <c r="E7" s="11"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="13"/>
+      <c r="G7" s="11"/>
       <c r="H7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3614,9 +3601,9 @@
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="13"/>
+      <c r="E8" s="11"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="13"/>
+      <c r="G8" s="11"/>
       <c r="H8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3624,9 +3611,9 @@
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
-      <c r="E9" s="13"/>
+      <c r="E9" s="11"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="13"/>
+      <c r="G9" s="11"/>
       <c r="H9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3634,9 +3621,9 @@
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="13"/>
+      <c r="E10" s="11"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="13"/>
+      <c r="G10" s="11"/>
       <c r="H10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3644,9 +3631,9 @@
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="13"/>
+      <c r="E11" s="11"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="13"/>
+      <c r="G11" s="11"/>
       <c r="H11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3654,9 +3641,9 @@
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="13"/>
+      <c r="E12" s="11"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="13"/>
+      <c r="G12" s="11"/>
       <c r="H12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3664,9 +3651,9 @@
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="13"/>
+      <c r="E13" s="11"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="13"/>
+      <c r="G13" s="11"/>
       <c r="H13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3674,9 +3661,9 @@
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="13"/>
+      <c r="E14" s="11"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="13"/>
+      <c r="G14" s="11"/>
       <c r="H14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3684,9 +3671,9 @@
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
-      <c r="E15" s="13"/>
+      <c r="E15" s="11"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="13"/>
+      <c r="G15" s="11"/>
       <c r="H15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3694,9 +3681,9 @@
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="13"/>
+      <c r="E16" s="11"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="13"/>
+      <c r="G16" s="11"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3704,9 +3691,9 @@
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="13"/>
+      <c r="E17" s="11"/>
       <c r="F17" s="5"/>
-      <c r="G17" s="13"/>
+      <c r="G17" s="11"/>
       <c r="H17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3714,9 +3701,9 @@
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="13"/>
+      <c r="E18" s="11"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="13"/>
+      <c r="G18" s="11"/>
       <c r="H18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3724,9 +3711,9 @@
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="13"/>
+      <c r="E19" s="11"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="13"/>
+      <c r="G19" s="11"/>
       <c r="H19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3734,9 +3721,9 @@
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
-      <c r="E20" s="13"/>
+      <c r="E20" s="11"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="13"/>
+      <c r="G20" s="11"/>
       <c r="H20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3744,9 +3731,9 @@
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="13"/>
+      <c r="E21" s="11"/>
       <c r="F21" s="5"/>
-      <c r="G21" s="13"/>
+      <c r="G21" s="11"/>
       <c r="H21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3754,9 +3741,9 @@
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
-      <c r="E22" s="13"/>
+      <c r="E22" s="11"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="13"/>
+      <c r="G22" s="11"/>
       <c r="H22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3764,9 +3751,9 @@
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
-      <c r="E23" s="13"/>
+      <c r="E23" s="11"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="13"/>
+      <c r="G23" s="11"/>
       <c r="H23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3774,9 +3761,9 @@
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="13"/>
+      <c r="E24" s="11"/>
       <c r="F24" s="5"/>
-      <c r="G24" s="13"/>
+      <c r="G24" s="11"/>
       <c r="H24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3784,9 +3771,9 @@
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
-      <c r="E25" s="13"/>
+      <c r="E25" s="11"/>
       <c r="F25" s="5"/>
-      <c r="G25" s="13"/>
+      <c r="G25" s="11"/>
       <c r="H25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3794,9 +3781,9 @@
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
-      <c r="E26" s="13"/>
+      <c r="E26" s="11"/>
       <c r="F26" s="5"/>
-      <c r="G26" s="13"/>
+      <c r="G26" s="11"/>
       <c r="H26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3804,9 +3791,9 @@
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="13"/>
+      <c r="E27" s="11"/>
       <c r="F27" s="5"/>
-      <c r="G27" s="13"/>
+      <c r="G27" s="11"/>
       <c r="H27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3814,9 +3801,9 @@
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
-      <c r="E28" s="13"/>
+      <c r="E28" s="11"/>
       <c r="F28" s="5"/>
-      <c r="G28" s="13"/>
+      <c r="G28" s="11"/>
       <c r="H28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3824,9 +3811,9 @@
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
-      <c r="E29" s="13"/>
+      <c r="E29" s="11"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="13"/>
+      <c r="G29" s="11"/>
       <c r="H29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3834,9 +3821,9 @@
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="13"/>
+      <c r="E30" s="11"/>
       <c r="F30" s="5"/>
-      <c r="G30" s="13"/>
+      <c r="G30" s="11"/>
       <c r="H30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3844,9 +3831,9 @@
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="13"/>
+      <c r="E31" s="11"/>
       <c r="F31" s="5"/>
-      <c r="G31" s="13"/>
+      <c r="G31" s="11"/>
       <c r="H31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3854,9 +3841,9 @@
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="13"/>
+      <c r="E32" s="11"/>
       <c r="F32" s="5"/>
-      <c r="G32" s="13"/>
+      <c r="G32" s="11"/>
       <c r="H32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3864,9 +3851,9 @@
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
-      <c r="E33" s="13"/>
+      <c r="E33" s="11"/>
       <c r="F33" s="5"/>
-      <c r="G33" s="13"/>
+      <c r="G33" s="11"/>
       <c r="H33" s="5"/>
     </row>
   </sheetData>
@@ -3956,7 +3943,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="129.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="11" t="s">
         <v>120</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -3977,7 +3964,7 @@
       <c r="G4" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="11" t="s">
         <v>127</v>
       </c>
       <c r="I4" s="5" t="s">
@@ -3985,311 +3972,311 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="13"/>
+      <c r="H5" s="11"/>
       <c r="I5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="13"/>
+      <c r="H6" s="11"/>
       <c r="I6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="13"/>
+      <c r="H7" s="11"/>
       <c r="I7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="13"/>
+      <c r="H8" s="11"/>
       <c r="I8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="13"/>
+      <c r="H9" s="11"/>
       <c r="I9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="13"/>
+      <c r="H10" s="11"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="13"/>
+      <c r="H11" s="11"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="13"/>
+      <c r="H12" s="11"/>
       <c r="I12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="13"/>
+      <c r="H13" s="11"/>
       <c r="I13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="13"/>
+      <c r="H14" s="11"/>
       <c r="I14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="13"/>
+      <c r="H15" s="11"/>
       <c r="I15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="13"/>
+      <c r="H16" s="11"/>
       <c r="I16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="13"/>
+      <c r="H17" s="11"/>
       <c r="I17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
-      <c r="H18" s="13"/>
+      <c r="H18" s="11"/>
       <c r="I18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="13"/>
+      <c r="H19" s="11"/>
       <c r="I19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="13"/>
+      <c r="H20" s="11"/>
       <c r="I20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="13"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
-      <c r="H21" s="13"/>
+      <c r="H21" s="11"/>
       <c r="I21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="13"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
-      <c r="H22" s="13"/>
+      <c r="H22" s="11"/>
       <c r="I22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="13"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="13"/>
+      <c r="H23" s="11"/>
       <c r="I23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="13"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="13"/>
+      <c r="H24" s="11"/>
       <c r="I24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="13"/>
+      <c r="A25" s="11"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="13"/>
+      <c r="H25" s="11"/>
       <c r="I25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="13"/>
+      <c r="A26" s="11"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
-      <c r="H26" s="13"/>
+      <c r="H26" s="11"/>
       <c r="I26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="13"/>
+      <c r="A27" s="11"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
-      <c r="H27" s="13"/>
+      <c r="H27" s="11"/>
       <c r="I27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="13"/>
+      <c r="A28" s="11"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
-      <c r="H28" s="13"/>
+      <c r="H28" s="11"/>
       <c r="I28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="13"/>
+      <c r="A29" s="11"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
-      <c r="H29" s="13"/>
+      <c r="H29" s="11"/>
       <c r="I29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="13"/>
+      <c r="A30" s="11"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
-      <c r="H30" s="13"/>
+      <c r="H30" s="11"/>
       <c r="I30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="13"/>
+      <c r="A31" s="11"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
-      <c r="H31" s="13"/>
+      <c r="H31" s="11"/>
       <c r="I31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="13"/>
+      <c r="A32" s="11"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
-      <c r="H32" s="13"/>
+      <c r="H32" s="11"/>
       <c r="I32" s="5"/>
     </row>
   </sheetData>
@@ -4394,7 +4381,7 @@
       <c r="I7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="12" t="s">
         <v>140</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -4423,7 +4410,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -4434,7 +4421,7 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="14"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -4445,7 +4432,7 @@
       <c r="I10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="14"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -4456,7 +4443,7 @@
       <c r="I11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="14"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -4467,7 +4454,7 @@
       <c r="I12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -4478,7 +4465,7 @@
       <c r="I13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -4489,7 +4476,7 @@
       <c r="I14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="14"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -4500,7 +4487,7 @@
       <c r="I15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="14"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -4511,7 +4498,7 @@
       <c r="I16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="14"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -4522,7 +4509,7 @@
       <c r="I17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -4533,7 +4520,7 @@
       <c r="I18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -4544,7 +4531,7 @@
       <c r="I19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -4555,7 +4542,7 @@
       <c r="I20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="14"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -4566,7 +4553,7 @@
       <c r="I21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="14"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -4577,7 +4564,7 @@
       <c r="I22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="14"/>
+      <c r="A23" s="12"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -4588,7 +4575,7 @@
       <c r="I23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="14"/>
+      <c r="A24" s="12"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -4599,7 +4586,7 @@
       <c r="I24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="14"/>
+      <c r="A25" s="12"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -4610,7 +4597,7 @@
       <c r="I25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="14"/>
+      <c r="A26" s="12"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -4621,7 +4608,7 @@
       <c r="I26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="14"/>
+      <c r="A27" s="12"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -4632,7 +4619,7 @@
       <c r="I27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="14"/>
+      <c r="A28" s="12"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -4643,7 +4630,7 @@
       <c r="I28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="14"/>
+      <c r="A29" s="12"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -4654,7 +4641,7 @@
       <c r="I29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="14"/>
+      <c r="A30" s="12"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -4665,7 +4652,7 @@
       <c r="I30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="14"/>
+      <c r="A31" s="12"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -4676,7 +4663,7 @@
       <c r="I31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="14"/>
+      <c r="A32" s="12"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -4687,7 +4674,7 @@
       <c r="I32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="14"/>
+      <c r="A33" s="12"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -4698,7 +4685,7 @@
       <c r="I33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="14"/>
+      <c r="A34" s="12"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -4709,7 +4696,7 @@
       <c r="I34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="14"/>
+      <c r="A35" s="12"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -4720,7 +4707,7 @@
       <c r="I35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="14"/>
+      <c r="A36" s="12"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -4808,7 +4795,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="11" t="s">
         <v>157</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -4840,7 +4827,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -4852,7 +4839,7 @@
       <c r="J10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -4864,7 +4851,7 @@
       <c r="J11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -4876,7 +4863,7 @@
       <c r="J12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -4888,7 +4875,7 @@
       <c r="J13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -4900,7 +4887,7 @@
       <c r="J14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -4912,7 +4899,7 @@
       <c r="J15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -4924,7 +4911,7 @@
       <c r="J16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -4936,7 +4923,7 @@
       <c r="J17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -4948,7 +4935,7 @@
       <c r="J18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -4960,7 +4947,7 @@
       <c r="J19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -4972,7 +4959,7 @@
       <c r="J20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="13"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -4984,7 +4971,7 @@
       <c r="J21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="13"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -4996,7 +4983,7 @@
       <c r="J22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="13"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -5008,7 +4995,7 @@
       <c r="J23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="13"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -5020,7 +5007,7 @@
       <c r="J24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="13"/>
+      <c r="A25" s="11"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -5032,7 +5019,7 @@
       <c r="J25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="13"/>
+      <c r="A26" s="11"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -5044,7 +5031,7 @@
       <c r="J26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="13"/>
+      <c r="A27" s="11"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -5056,7 +5043,7 @@
       <c r="J27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="13"/>
+      <c r="A28" s="11"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -5068,7 +5055,7 @@
       <c r="J28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="13"/>
+      <c r="A29" s="11"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -5080,7 +5067,7 @@
       <c r="J29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="13"/>
+      <c r="A30" s="11"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -5092,7 +5079,7 @@
       <c r="J30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="13"/>
+      <c r="A31" s="11"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -5104,7 +5091,7 @@
       <c r="J31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="13"/>
+      <c r="A32" s="11"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -5116,7 +5103,7 @@
       <c r="J32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="13"/>
+      <c r="A33" s="11"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -5128,7 +5115,7 @@
       <c r="J33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="13"/>
+      <c r="A34" s="11"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -5140,7 +5127,7 @@
       <c r="J34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="13"/>
+      <c r="A35" s="11"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -5152,7 +5139,7 @@
       <c r="J35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="13"/>
+      <c r="A36" s="11"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -5164,7 +5151,7 @@
       <c r="J36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="13"/>
+      <c r="A37" s="11"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -5272,7 +5259,7 @@
       <c r="B8" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="13" t="s">
         <v>176</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -5307,7 +5294,7 @@
       <c r="A9" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="11" t="s">
         <v>182</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -5334,7 +5321,7 @@
       <c r="J9" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="K9" s="13" t="s">
+      <c r="K9" s="11" t="s">
         <v>191</v>
       </c>
       <c r="L9" s="5" t="s">
@@ -5343,7 +5330,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10"/>
-      <c r="B10" s="13"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -5352,12 +5339,12 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="13"/>
+      <c r="K10" s="11"/>
       <c r="L10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10"/>
-      <c r="B11" s="13"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -5366,12 +5353,12 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="13"/>
+      <c r="K11" s="11"/>
       <c r="L11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10"/>
-      <c r="B12" s="13"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -5380,12 +5367,12 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="13"/>
+      <c r="K12" s="11"/>
       <c r="L12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10"/>
-      <c r="B13" s="13"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -5394,12 +5381,12 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="13"/>
+      <c r="K13" s="11"/>
       <c r="L13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10"/>
-      <c r="B14" s="13"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -5408,12 +5395,12 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="13"/>
+      <c r="K14" s="11"/>
       <c r="L14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10"/>
-      <c r="B15" s="13"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -5422,12 +5409,12 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
-      <c r="K15" s="13"/>
+      <c r="K15" s="11"/>
       <c r="L15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10"/>
-      <c r="B16" s="13"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -5436,12 +5423,12 @@
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
-      <c r="K16" s="13"/>
+      <c r="K16" s="11"/>
       <c r="L16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10"/>
-      <c r="B17" s="13"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -5450,12 +5437,12 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
-      <c r="K17" s="13"/>
+      <c r="K17" s="11"/>
       <c r="L17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10"/>
-      <c r="B18" s="13"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -5464,12 +5451,12 @@
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
-      <c r="K18" s="13"/>
+      <c r="K18" s="11"/>
       <c r="L18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
-      <c r="B19" s="13"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -5478,12 +5465,12 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
-      <c r="K19" s="13"/>
+      <c r="K19" s="11"/>
       <c r="L19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
-      <c r="B20" s="13"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -5492,12 +5479,12 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
-      <c r="K20" s="13"/>
+      <c r="K20" s="11"/>
       <c r="L20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
-      <c r="B21" s="13"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -5506,12 +5493,12 @@
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
-      <c r="K21" s="13"/>
+      <c r="K21" s="11"/>
       <c r="L21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
-      <c r="B22" s="13"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -5520,12 +5507,12 @@
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
-      <c r="K22" s="13"/>
+      <c r="K22" s="11"/>
       <c r="L22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
-      <c r="B23" s="13"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
@@ -5534,12 +5521,12 @@
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
-      <c r="K23" s="13"/>
+      <c r="K23" s="11"/>
       <c r="L23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10"/>
-      <c r="B24" s="13"/>
+      <c r="B24" s="11"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
@@ -5548,12 +5535,12 @@
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
-      <c r="K24" s="13"/>
+      <c r="K24" s="11"/>
       <c r="L24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
-      <c r="B25" s="13"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
@@ -5562,12 +5549,12 @@
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
-      <c r="K25" s="13"/>
+      <c r="K25" s="11"/>
       <c r="L25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
-      <c r="B26" s="13"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
@@ -5576,12 +5563,12 @@
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
-      <c r="K26" s="13"/>
+      <c r="K26" s="11"/>
       <c r="L26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
-      <c r="B27" s="13"/>
+      <c r="B27" s="11"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
@@ -5590,12 +5577,12 @@
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
-      <c r="K27" s="13"/>
+      <c r="K27" s="11"/>
       <c r="L27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
-      <c r="B28" s="13"/>
+      <c r="B28" s="11"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
@@ -5604,12 +5591,12 @@
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
-      <c r="K28" s="13"/>
+      <c r="K28" s="11"/>
       <c r="L28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
-      <c r="B29" s="13"/>
+      <c r="B29" s="11"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
@@ -5618,12 +5605,12 @@
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
-      <c r="K29" s="13"/>
+      <c r="K29" s="11"/>
       <c r="L29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="10"/>
-      <c r="B30" s="13"/>
+      <c r="B30" s="11"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
@@ -5632,12 +5619,12 @@
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
-      <c r="K30" s="13"/>
+      <c r="K30" s="11"/>
       <c r="L30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10"/>
-      <c r="B31" s="13"/>
+      <c r="B31" s="11"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
@@ -5646,12 +5633,12 @@
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
-      <c r="K31" s="13"/>
+      <c r="K31" s="11"/>
       <c r="L31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="10"/>
-      <c r="B32" s="13"/>
+      <c r="B32" s="11"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
@@ -5660,12 +5647,12 @@
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
-      <c r="K32" s="13"/>
+      <c r="K32" s="11"/>
       <c r="L32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="10"/>
-      <c r="B33" s="13"/>
+      <c r="B33" s="11"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
@@ -5674,12 +5661,12 @@
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
-      <c r="K33" s="13"/>
+      <c r="K33" s="11"/>
       <c r="L33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="10"/>
-      <c r="B34" s="13"/>
+      <c r="B34" s="11"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
@@ -5688,12 +5675,12 @@
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
-      <c r="K34" s="13"/>
+      <c r="K34" s="11"/>
       <c r="L34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="10"/>
-      <c r="B35" s="13"/>
+      <c r="B35" s="11"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
@@ -5702,12 +5689,12 @@
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
-      <c r="K35" s="13"/>
+      <c r="K35" s="11"/>
       <c r="L35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="10"/>
-      <c r="B36" s="13"/>
+      <c r="B36" s="11"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
@@ -5716,12 +5703,12 @@
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
-      <c r="K36" s="13"/>
+      <c r="K36" s="11"/>
       <c r="L36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="10"/>
-      <c r="B37" s="13"/>
+      <c r="B37" s="11"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
@@ -5730,7 +5717,7 @@
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
-      <c r="K37" s="13"/>
+      <c r="K37" s="11"/>
       <c r="L37" s="5"/>
     </row>
   </sheetData>
@@ -5843,10 +5830,10 @@
       <c r="A10" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="13" t="s">
         <v>199</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -5881,7 +5868,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="143.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="11" t="s">
         <v>206</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -5914,7 +5901,7 @@
       <c r="K11" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="L11" s="13" t="s">
+      <c r="L11" s="11" t="s">
         <v>217</v>
       </c>
       <c r="M11" s="5" t="s">
@@ -5922,7 +5909,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -5933,11 +5920,11 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
-      <c r="L12" s="13"/>
+      <c r="L12" s="11"/>
       <c r="M12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -5948,11 +5935,11 @@
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="13"/>
+      <c r="L13" s="11"/>
       <c r="M13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -5963,11 +5950,11 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
-      <c r="L14" s="13"/>
+      <c r="L14" s="11"/>
       <c r="M14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -5978,11 +5965,11 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
-      <c r="L15" s="13"/>
+      <c r="L15" s="11"/>
       <c r="M15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -5993,11 +5980,11 @@
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
-      <c r="L16" s="13"/>
+      <c r="L16" s="11"/>
       <c r="M16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -6008,11 +5995,11 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
-      <c r="L17" s="13"/>
+      <c r="L17" s="11"/>
       <c r="M17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -6023,11 +6010,11 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
-      <c r="L18" s="13"/>
+      <c r="L18" s="11"/>
       <c r="M18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -6038,11 +6025,11 @@
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
-      <c r="L19" s="13"/>
+      <c r="L19" s="11"/>
       <c r="M19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -6053,11 +6040,11 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
-      <c r="L20" s="13"/>
+      <c r="L20" s="11"/>
       <c r="M20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="13"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -6068,11 +6055,11 @@
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
-      <c r="L21" s="13"/>
+      <c r="L21" s="11"/>
       <c r="M21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="13"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -6083,11 +6070,11 @@
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="13"/>
+      <c r="L22" s="11"/>
       <c r="M22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="13"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -6098,11 +6085,11 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
-      <c r="L23" s="13"/>
+      <c r="L23" s="11"/>
       <c r="M23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="13"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -6113,11 +6100,11 @@
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
-      <c r="L24" s="13"/>
+      <c r="L24" s="11"/>
       <c r="M24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="13"/>
+      <c r="A25" s="11"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -6128,11 +6115,11 @@
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
-      <c r="L25" s="13"/>
+      <c r="L25" s="11"/>
       <c r="M25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="13"/>
+      <c r="A26" s="11"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -6143,11 +6130,11 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
-      <c r="L26" s="13"/>
+      <c r="L26" s="11"/>
       <c r="M26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="13"/>
+      <c r="A27" s="11"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -6158,11 +6145,11 @@
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
-      <c r="L27" s="13"/>
+      <c r="L27" s="11"/>
       <c r="M27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="13"/>
+      <c r="A28" s="11"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -6173,11 +6160,11 @@
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
-      <c r="L28" s="13"/>
+      <c r="L28" s="11"/>
       <c r="M28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="13"/>
+      <c r="A29" s="11"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -6188,11 +6175,11 @@
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
-      <c r="L29" s="13"/>
+      <c r="L29" s="11"/>
       <c r="M29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="13"/>
+      <c r="A30" s="11"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -6203,11 +6190,11 @@
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
-      <c r="L30" s="13"/>
+      <c r="L30" s="11"/>
       <c r="M30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="13"/>
+      <c r="A31" s="11"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -6218,11 +6205,11 @@
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
-      <c r="L31" s="13"/>
+      <c r="L31" s="11"/>
       <c r="M31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="13"/>
+      <c r="A32" s="11"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -6233,11 +6220,11 @@
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
-      <c r="L32" s="13"/>
+      <c r="L32" s="11"/>
       <c r="M32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="13"/>
+      <c r="A33" s="11"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -6248,11 +6235,11 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
-      <c r="L33" s="13"/>
+      <c r="L33" s="11"/>
       <c r="M33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="13"/>
+      <c r="A34" s="11"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -6263,11 +6250,11 @@
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
-      <c r="L34" s="13"/>
+      <c r="L34" s="11"/>
       <c r="M34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="13"/>
+      <c r="A35" s="11"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -6278,11 +6265,11 @@
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
-      <c r="L35" s="13"/>
+      <c r="L35" s="11"/>
       <c r="M35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="13"/>
+      <c r="A36" s="11"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -6293,11 +6280,11 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
-      <c r="L36" s="13"/>
+      <c r="L36" s="11"/>
       <c r="M36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="13"/>
+      <c r="A37" s="11"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -6308,11 +6295,11 @@
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
-      <c r="L37" s="13"/>
+      <c r="L37" s="11"/>
       <c r="M37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="13"/>
+      <c r="A38" s="11"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -6323,11 +6310,11 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
-      <c r="L38" s="13"/>
+      <c r="L38" s="11"/>
       <c r="M38" s="5"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="13"/>
+      <c r="A39" s="11"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -6338,7 +6325,7 @@
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
-      <c r="L39" s="13"/>
+      <c r="L39" s="11"/>
       <c r="M39" s="5"/>
     </row>
   </sheetData>
@@ -6510,7 +6497,7 @@
       <c r="B17" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="13" t="s">
         <v>176</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -6537,13 +6524,13 @@
       <c r="K17" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="L17" s="15" t="s">
+      <c r="L17" s="13" t="s">
         <v>246</v>
       </c>
       <c r="M17" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="N17" s="15" t="s">
+      <c r="N17" s="13" t="s">
         <v>248</v>
       </c>
       <c r="O17" s="3" t="s">
@@ -6560,7 +6547,7 @@
       <c r="A18" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="11" t="s">
         <v>251</v>
       </c>
       <c r="C18" s="5" t="s">
@@ -6602,7 +6589,7 @@
       <c r="O18" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="P18" s="13" t="s">
+      <c r="P18" s="11" t="s">
         <v>265</v>
       </c>
       <c r="Q18" s="5" t="s">
@@ -6611,7 +6598,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
-      <c r="B19" s="13"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -6625,12 +6612,12 @@
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
-      <c r="P19" s="13"/>
+      <c r="P19" s="11"/>
       <c r="Q19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
-      <c r="B20" s="13"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -6644,12 +6631,12 @@
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
-      <c r="P20" s="13"/>
+      <c r="P20" s="11"/>
       <c r="Q20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
-      <c r="B21" s="13"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -6663,12 +6650,12 @@
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
-      <c r="P21" s="13"/>
+      <c r="P21" s="11"/>
       <c r="Q21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
-      <c r="B22" s="13"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -6682,12 +6669,12 @@
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
-      <c r="P22" s="13"/>
+      <c r="P22" s="11"/>
       <c r="Q22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
-      <c r="B23" s="13"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
@@ -6701,12 +6688,12 @@
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
-      <c r="P23" s="13"/>
+      <c r="P23" s="11"/>
       <c r="Q23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10"/>
-      <c r="B24" s="13"/>
+      <c r="B24" s="11"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
@@ -6720,12 +6707,12 @@
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
-      <c r="P24" s="13"/>
+      <c r="P24" s="11"/>
       <c r="Q24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
-      <c r="B25" s="13"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
@@ -6739,12 +6726,12 @@
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
-      <c r="P25" s="13"/>
+      <c r="P25" s="11"/>
       <c r="Q25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
-      <c r="B26" s="13"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
@@ -6758,12 +6745,12 @@
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
-      <c r="P26" s="13"/>
+      <c r="P26" s="11"/>
       <c r="Q26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
-      <c r="B27" s="13"/>
+      <c r="B27" s="11"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
@@ -6777,12 +6764,12 @@
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
-      <c r="P27" s="13"/>
+      <c r="P27" s="11"/>
       <c r="Q27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
-      <c r="B28" s="13"/>
+      <c r="B28" s="11"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
@@ -6796,12 +6783,12 @@
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
-      <c r="P28" s="13"/>
+      <c r="P28" s="11"/>
       <c r="Q28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
-      <c r="B29" s="13"/>
+      <c r="B29" s="11"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
@@ -6815,12 +6802,12 @@
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
-      <c r="P29" s="13"/>
+      <c r="P29" s="11"/>
       <c r="Q29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="10"/>
-      <c r="B30" s="13"/>
+      <c r="B30" s="11"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
@@ -6834,12 +6821,12 @@
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
-      <c r="P30" s="13"/>
+      <c r="P30" s="11"/>
       <c r="Q30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10"/>
-      <c r="B31" s="13"/>
+      <c r="B31" s="11"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
@@ -6853,12 +6840,12 @@
       <c r="M31" s="5"/>
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
-      <c r="P31" s="13"/>
+      <c r="P31" s="11"/>
       <c r="Q31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="10"/>
-      <c r="B32" s="13"/>
+      <c r="B32" s="11"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
@@ -6872,12 +6859,12 @@
       <c r="M32" s="5"/>
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
-      <c r="P32" s="13"/>
+      <c r="P32" s="11"/>
       <c r="Q32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="10"/>
-      <c r="B33" s="13"/>
+      <c r="B33" s="11"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
@@ -6891,12 +6878,12 @@
       <c r="M33" s="5"/>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
-      <c r="P33" s="13"/>
+      <c r="P33" s="11"/>
       <c r="Q33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="10"/>
-      <c r="B34" s="13"/>
+      <c r="B34" s="11"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
@@ -6910,12 +6897,12 @@
       <c r="M34" s="5"/>
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
-      <c r="P34" s="13"/>
+      <c r="P34" s="11"/>
       <c r="Q34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="10"/>
-      <c r="B35" s="13"/>
+      <c r="B35" s="11"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
@@ -6929,12 +6916,12 @@
       <c r="M35" s="5"/>
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
-      <c r="P35" s="13"/>
+      <c r="P35" s="11"/>
       <c r="Q35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="10"/>
-      <c r="B36" s="13"/>
+      <c r="B36" s="11"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
@@ -6948,12 +6935,12 @@
       <c r="M36" s="5"/>
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
-      <c r="P36" s="13"/>
+      <c r="P36" s="11"/>
       <c r="Q36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="10"/>
-      <c r="B37" s="13"/>
+      <c r="B37" s="11"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
@@ -6967,12 +6954,12 @@
       <c r="M37" s="5"/>
       <c r="N37" s="5"/>
       <c r="O37" s="5"/>
-      <c r="P37" s="13"/>
+      <c r="P37" s="11"/>
       <c r="Q37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="10"/>
-      <c r="B38" s="13"/>
+      <c r="B38" s="11"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
@@ -6986,12 +6973,12 @@
       <c r="M38" s="5"/>
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
-      <c r="P38" s="13"/>
+      <c r="P38" s="11"/>
       <c r="Q38" s="5"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="10"/>
-      <c r="B39" s="13"/>
+      <c r="B39" s="11"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
@@ -7005,12 +6992,12 @@
       <c r="M39" s="5"/>
       <c r="N39" s="5"/>
       <c r="O39" s="5"/>
-      <c r="P39" s="13"/>
+      <c r="P39" s="11"/>
       <c r="Q39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="10"/>
-      <c r="B40" s="13"/>
+      <c r="B40" s="11"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
@@ -7024,12 +7011,12 @@
       <c r="M40" s="5"/>
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
-      <c r="P40" s="13"/>
+      <c r="P40" s="11"/>
       <c r="Q40" s="5"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="10"/>
-      <c r="B41" s="13"/>
+      <c r="B41" s="11"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
@@ -7043,12 +7030,12 @@
       <c r="M41" s="5"/>
       <c r="N41" s="5"/>
       <c r="O41" s="5"/>
-      <c r="P41" s="13"/>
+      <c r="P41" s="11"/>
       <c r="Q41" s="5"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="10"/>
-      <c r="B42" s="13"/>
+      <c r="B42" s="11"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
@@ -7062,12 +7049,12 @@
       <c r="M42" s="5"/>
       <c r="N42" s="5"/>
       <c r="O42" s="5"/>
-      <c r="P42" s="13"/>
+      <c r="P42" s="11"/>
       <c r="Q42" s="5"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="10"/>
-      <c r="B43" s="13"/>
+      <c r="B43" s="11"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
@@ -7081,12 +7068,12 @@
       <c r="M43" s="5"/>
       <c r="N43" s="5"/>
       <c r="O43" s="5"/>
-      <c r="P43" s="13"/>
+      <c r="P43" s="11"/>
       <c r="Q43" s="5"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="10"/>
-      <c r="B44" s="13"/>
+      <c r="B44" s="11"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
@@ -7100,12 +7087,12 @@
       <c r="M44" s="5"/>
       <c r="N44" s="5"/>
       <c r="O44" s="5"/>
-      <c r="P44" s="13"/>
+      <c r="P44" s="11"/>
       <c r="Q44" s="5"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="10"/>
-      <c r="B45" s="13"/>
+      <c r="B45" s="11"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
@@ -7119,12 +7106,12 @@
       <c r="M45" s="5"/>
       <c r="N45" s="5"/>
       <c r="O45" s="5"/>
-      <c r="P45" s="13"/>
+      <c r="P45" s="11"/>
       <c r="Q45" s="5"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="10"/>
-      <c r="B46" s="13"/>
+      <c r="B46" s="11"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
@@ -7138,7 +7125,7 @@
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
       <c r="O46" s="5"/>
-      <c r="P46" s="13"/>
+      <c r="P46" s="11"/>
       <c r="Q46" s="5"/>
     </row>
   </sheetData>
@@ -7239,10 +7226,10 @@
       <c r="A12" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="13" t="s">
         <v>275</v>
       </c>
       <c r="D12" s="9" t="s">
@@ -7253,7 +7240,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="11" t="s">
         <v>276</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -7262,7 +7249,7 @@
       <c r="C13" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="11" t="s">
         <v>279</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -7270,199 +7257,199 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="13"/>
+      <c r="D14" s="11"/>
       <c r="E14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="13"/>
+      <c r="D15" s="11"/>
       <c r="E15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="13"/>
+      <c r="D16" s="11"/>
       <c r="E16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
-      <c r="D17" s="13"/>
+      <c r="D17" s="11"/>
       <c r="E17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
-      <c r="D18" s="13"/>
+      <c r="D18" s="11"/>
       <c r="E18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="13"/>
+      <c r="D19" s="11"/>
       <c r="E19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
-      <c r="D20" s="13"/>
+      <c r="D20" s="11"/>
       <c r="E20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="13"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
-      <c r="D21" s="13"/>
+      <c r="D21" s="11"/>
       <c r="E21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="13"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
-      <c r="D22" s="13"/>
+      <c r="D22" s="11"/>
       <c r="E22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="13"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
-      <c r="D23" s="13"/>
+      <c r="D23" s="11"/>
       <c r="E23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="13"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
-      <c r="D24" s="13"/>
+      <c r="D24" s="11"/>
       <c r="E24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="13"/>
+      <c r="A25" s="11"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
-      <c r="D25" s="13"/>
+      <c r="D25" s="11"/>
       <c r="E25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="13"/>
+      <c r="A26" s="11"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
-      <c r="D26" s="13"/>
+      <c r="D26" s="11"/>
       <c r="E26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="13"/>
+      <c r="A27" s="11"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
-      <c r="D27" s="13"/>
+      <c r="D27" s="11"/>
       <c r="E27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="13"/>
+      <c r="A28" s="11"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
-      <c r="D28" s="13"/>
+      <c r="D28" s="11"/>
       <c r="E28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="13"/>
+      <c r="A29" s="11"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
-      <c r="D29" s="13"/>
+      <c r="D29" s="11"/>
       <c r="E29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="13"/>
+      <c r="A30" s="11"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
-      <c r="D30" s="13"/>
+      <c r="D30" s="11"/>
       <c r="E30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="13"/>
+      <c r="A31" s="11"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
-      <c r="D31" s="13"/>
+      <c r="D31" s="11"/>
       <c r="E31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="13"/>
+      <c r="A32" s="11"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
-      <c r="D32" s="13"/>
+      <c r="D32" s="11"/>
       <c r="E32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="13"/>
+      <c r="A33" s="11"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
-      <c r="D33" s="13"/>
+      <c r="D33" s="11"/>
       <c r="E33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="13"/>
+      <c r="A34" s="11"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
-      <c r="D34" s="13"/>
+      <c r="D34" s="11"/>
       <c r="E34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="13"/>
+      <c r="A35" s="11"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
-      <c r="D35" s="13"/>
+      <c r="D35" s="11"/>
       <c r="E35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="13"/>
+      <c r="A36" s="11"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
-      <c r="D36" s="13"/>
+      <c r="D36" s="11"/>
       <c r="E36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="13"/>
+      <c r="A37" s="11"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="13"/>
+      <c r="D37" s="11"/>
       <c r="E37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="13"/>
+      <c r="A38" s="11"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="13"/>
+      <c r="D38" s="11"/>
       <c r="E38" s="5"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="13"/>
+      <c r="A39" s="11"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
-      <c r="D39" s="13"/>
+      <c r="D39" s="11"/>
       <c r="E39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="13"/>
+      <c r="A40" s="11"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
-      <c r="D40" s="13"/>
+      <c r="D40" s="11"/>
       <c r="E40" s="5"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="13"/>
+      <c r="A41" s="11"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
-      <c r="D41" s="13"/>
+      <c r="D41" s="11"/>
       <c r="E41" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data-model: Tweaks to project
https://github.com/INDIGO-Initiative/database-app/issues/10
https://github.com/INDIGO-Initiative/database-app/issues/8
https://github.com/INDIGO-Initiative/database-app/issues/7
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/project-public.xlsx
+++ b/indigo/spreadsheetform_guides/project-public.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="348">
   <si>
     <t xml:space="preserve">Indigo Project ID</t>
   </si>
@@ -323,6 +323,9 @@
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:SINGLE:changes_to_project_due_to_covid19/source_ids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:notes/value</t>
   </si>
   <si>
     <t xml:space="preserve">Meta</t>
@@ -629,11 +632,19 @@
     <t xml:space="preserve">Overall</t>
   </si>
   <si>
+    <t xml:space="preserve">Maximum potential Outcome payment</t>
+  </si>
+  <si>
     <t xml:space="preserve">Alterations to payment commitment</t>
   </si>
   <si>
-    <t xml:space="preserve">Maximum potential
- Outcome payment</t>
+    <t xml:space="preserve">Currency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amount in USD</t>
   </si>
   <si>
     <t xml:space="preserve">Result type</t>
@@ -645,22 +656,19 @@
     <t xml:space="preserve">Period end</t>
   </si>
   <si>
-    <t xml:space="preserve">Currency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amount in USD</t>
-  </si>
-  <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_payment_commitments:organisation_id/value</t>
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_payment_commitments:organisation_role_category/value</t>
   </si>
   <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_payment_commitments:maximum_potential_outcome_payment/value</t>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_payment_commitments:maximum_potential_outcome_payment/currency/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_payment_commitments:maximum_potential_outcome_payment/amount/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_payment_commitments:maximum_potential_outcome_payment/amount_usd/value</t>
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_payment_commitments:result_type/value</t>
@@ -1366,7 +1374,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:F66"/>
+  <dimension ref="A2:F68"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1897,6 +1905,15 @@
       </c>
       <c r="D66" s="5" t="s">
         <v>96</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B68" s="4"/>
+      <c r="C68" s="5" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1938,44 +1955,44 @@
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I3" s="6" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I4" s="6" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I5" s="6" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I6" s="6" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E7" s="6" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E8" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1990,44 +2007,44 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>28</v>
@@ -2035,40 +2052,40 @@
     </row>
     <row r="11" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2506,18 +2523,18 @@
   <sheetData>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="6" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="6" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2533,47 +2550,47 @@
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="M8" s="3" t="s">
         <v>28</v>
@@ -2590,53 +2607,53 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="9" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="L9" s="9"/>
       <c r="M9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3093,17 +3110,17 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>28</v>
@@ -3111,13 +3128,13 @@
     </row>
     <row r="4" customFormat="false" ht="100.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3293,17 +3310,17 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>28</v>
@@ -3311,13 +3328,13 @@
     </row>
     <row r="4" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3507,32 +3524,32 @@
       <c r="E2" s="9"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>28</v>
@@ -3544,7 +3561,7 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="9"/>
@@ -3552,28 +3569,28 @@
     </row>
     <row r="5" customFormat="false" ht="101.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3898,45 +3915,45 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9"/>
       <c r="B2" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>28</v>
@@ -3944,31 +3961,31 @@
     </row>
     <row r="4" customFormat="false" ht="129.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4320,51 +4337,51 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4372,7 +4389,7 @@
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -4382,31 +4399,31 @@
     </row>
     <row r="8" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4746,19 +4763,19 @@
   <sheetData>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -4767,63 +4784,63 @@
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9"/>
       <c r="B8" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5206,27 +5223,27 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="6" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="6" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5235,56 +5252,56 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>69</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>177</v>
-      </c>
       <c r="H8" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>28</v>
@@ -5292,40 +5309,40 @@
     </row>
     <row r="9" customFormat="false" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5742,10 +5759,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:N39"/>
+  <dimension ref="A2:P39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N7" activeCellId="0" sqref="N7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5753,159 +5770,177 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="28.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.94"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="23.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.94"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="6" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="6" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="6" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="D7" s="6" t="s">
         <v>196</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>197</v>
+        <v>155</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3" t="s">
-        <v>198</v>
-      </c>
+      <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3" t="s">
-        <v>97</v>
+        <v>200</v>
       </c>
       <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-    </row>
-    <row r="10" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N9" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>199</v>
+        <v>177</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>201</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="J10" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="K10" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="K10" s="3" t="s">
+      <c r="L10" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="L10" s="9" t="s">
-        <v>104</v>
-      </c>
       <c r="M10" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="O10" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="143.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="158.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="L11" s="11" t="s">
         <v>217</v>
       </c>
+      <c r="L11" s="5" t="s">
+        <v>218</v>
+      </c>
       <c r="M11" s="5" t="s">
-        <v>218</v>
+        <v>219</v>
+      </c>
+      <c r="N11" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5920,8 +5955,10 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
-      <c r="L12" s="11"/>
+      <c r="L12" s="5"/>
       <c r="M12" s="5"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11"/>
@@ -5935,8 +5972,10 @@
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="11"/>
+      <c r="L13" s="5"/>
       <c r="M13" s="5"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11"/>
@@ -5950,8 +5989,10 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
-      <c r="L14" s="11"/>
+      <c r="L14" s="5"/>
       <c r="M14" s="5"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11"/>
@@ -5965,8 +6006,10 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
-      <c r="L15" s="11"/>
+      <c r="L15" s="5"/>
       <c r="M15" s="5"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11"/>
@@ -5980,8 +6023,10 @@
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
-      <c r="L16" s="11"/>
+      <c r="L16" s="5"/>
       <c r="M16" s="5"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11"/>
@@ -5995,8 +6040,10 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
-      <c r="L17" s="11"/>
+      <c r="L17" s="5"/>
       <c r="M17" s="5"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11"/>
@@ -6010,8 +6057,10 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
-      <c r="L18" s="11"/>
+      <c r="L18" s="5"/>
       <c r="M18" s="5"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11"/>
@@ -6025,8 +6074,10 @@
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
-      <c r="L19" s="11"/>
+      <c r="L19" s="5"/>
       <c r="M19" s="5"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="11"/>
@@ -6040,8 +6091,10 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
-      <c r="L20" s="11"/>
+      <c r="L20" s="5"/>
       <c r="M20" s="5"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11"/>
@@ -6055,8 +6108,10 @@
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
-      <c r="L21" s="11"/>
+      <c r="L21" s="5"/>
       <c r="M21" s="5"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11"/>
@@ -6070,8 +6125,10 @@
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="11"/>
+      <c r="L22" s="5"/>
       <c r="M22" s="5"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11"/>
@@ -6085,8 +6142,10 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
-      <c r="L23" s="11"/>
+      <c r="L23" s="5"/>
       <c r="M23" s="5"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="11"/>
@@ -6100,8 +6159,10 @@
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
-      <c r="L24" s="11"/>
+      <c r="L24" s="5"/>
       <c r="M24" s="5"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11"/>
@@ -6115,8 +6176,10 @@
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
-      <c r="L25" s="11"/>
+      <c r="L25" s="5"/>
       <c r="M25" s="5"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="11"/>
@@ -6130,8 +6193,10 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
-      <c r="L26" s="11"/>
+      <c r="L26" s="5"/>
       <c r="M26" s="5"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="11"/>
@@ -6145,8 +6210,10 @@
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
-      <c r="L27" s="11"/>
+      <c r="L27" s="5"/>
       <c r="M27" s="5"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11"/>
@@ -6160,8 +6227,10 @@
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
-      <c r="L28" s="11"/>
+      <c r="L28" s="5"/>
       <c r="M28" s="5"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="11"/>
@@ -6175,8 +6244,10 @@
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
-      <c r="L29" s="11"/>
+      <c r="L29" s="5"/>
       <c r="M29" s="5"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="11"/>
@@ -6190,8 +6261,10 @@
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
-      <c r="L30" s="11"/>
+      <c r="L30" s="5"/>
       <c r="M30" s="5"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="11"/>
@@ -6205,8 +6278,10 @@
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
-      <c r="L31" s="11"/>
+      <c r="L31" s="5"/>
       <c r="M31" s="5"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="11"/>
@@ -6220,8 +6295,10 @@
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
-      <c r="L32" s="11"/>
+      <c r="L32" s="5"/>
       <c r="M32" s="5"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="11"/>
@@ -6235,8 +6312,10 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
-      <c r="L33" s="11"/>
+      <c r="L33" s="5"/>
       <c r="M33" s="5"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="11"/>
@@ -6250,8 +6329,10 @@
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
-      <c r="L34" s="11"/>
+      <c r="L34" s="5"/>
       <c r="M34" s="5"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="11"/>
@@ -6265,8 +6346,10 @@
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
-      <c r="L35" s="11"/>
+      <c r="L35" s="5"/>
       <c r="M35" s="5"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="11"/>
@@ -6280,8 +6363,10 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
-      <c r="L36" s="11"/>
+      <c r="L36" s="5"/>
       <c r="M36" s="5"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="11"/>
@@ -6295,8 +6380,10 @@
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
-      <c r="L37" s="11"/>
+      <c r="L37" s="5"/>
       <c r="M37" s="5"/>
+      <c r="N37" s="11"/>
+      <c r="O37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="11"/>
@@ -6310,8 +6397,10 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
-      <c r="L38" s="11"/>
+      <c r="L38" s="5"/>
       <c r="M38" s="5"/>
+      <c r="N38" s="11"/>
+      <c r="O38" s="5"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="11"/>
@@ -6325,14 +6414,17 @@
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
-      <c r="L39" s="11"/>
+      <c r="L39" s="5"/>
       <c r="M39" s="5"/>
+      <c r="N39" s="11"/>
+      <c r="O39" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="L9:N9"/>
+  <mergeCells count="4">
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="N9:P9"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -6375,91 +6467,91 @@
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="6" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="6" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="6" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="6" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="6" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="6" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="6" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="6" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="6" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="6" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="6" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="6" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6467,7 +6559,7 @@
       <c r="B16" s="9"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -6476,68 +6568,68 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="O16" s="3"/>
       <c r="P16" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="L17" s="13" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="N17" s="13" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="P17" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="Q17" s="3" t="s">
         <v>28</v>
@@ -6545,55 +6637,55 @@
     </row>
     <row r="18" customFormat="false" ht="172.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="M18" s="5" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="O18" s="5" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="P18" s="11" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="Q18" s="5" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7169,47 +7261,47 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="6" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="6" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="6" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="6" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="6" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="6" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="6" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7217,23 +7309,23 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>28</v>
@@ -7241,19 +7333,19 @@
     </row>
     <row r="13" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
data-model: Tweaks to project, remove spaces from 2 keys
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/project-public.xlsx
+++ b/indigo/spreadsheetform_guides/project-public.xlsx
@@ -962,10 +962,10 @@
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_metrics:target_population/value</t>
   </si>
   <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_metrics:targeted_number_of_service_users _or_beneficiaries_total/value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_metrics:unit_type_of_targeted _service_users_or_beneficiaries/value</t>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_metrics:targeted_number_of_service_users_or_beneficiaries_total/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_metrics:unit_type_of_targeted_service_users_or_beneficiaries/value</t>
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_metrics:unit_description_of_service_user_or_beneficiaries/value</t>
@@ -1935,7 +1935,7 @@
   <dimension ref="A3:M39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
project: Add organisation name to spreadsheets
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/project-public.xlsx
+++ b/indigo/spreadsheetform_guides/project-public.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="349">
   <si>
     <t xml:space="preserve">Indigo Project ID</t>
   </si>
@@ -509,6 +509,9 @@
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:organisations:id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:organisations:name/value</t>
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:organisations:org-ids/company/value</t>
@@ -1137,7 +1140,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1159,7 +1162,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF2E75B6"/>
-        <bgColor rgb="FF0066CC"/>
+        <bgColor rgb="FF0066B3"/>
       </patternFill>
     </fill>
     <fill>
@@ -1196,6 +1199,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFC2E0AE"/>
         <bgColor rgb="FFE0EFD4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0066B3"/>
+        <bgColor rgb="FF008080"/>
       </patternFill>
     </fill>
   </fills>
@@ -1240,7 +1249,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1293,6 +1302,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1330,7 +1343,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FF0066B3"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -1955,33 +1968,33 @@
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I3" s="6" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I4" s="6" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I5" s="6" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I6" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E7" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1989,10 +2002,10 @@
         <v>155</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2014,34 +2027,34 @@
     </row>
     <row r="10" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>293</v>
-      </c>
-      <c r="C10" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>294</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="C10" s="14" t="s">
         <v>295</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="D10" s="14" t="s">
         <v>296</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="E10" s="14" t="s">
         <v>297</v>
       </c>
+      <c r="F10" s="14" t="s">
+        <v>298</v>
+      </c>
       <c r="G10" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="H10" s="13" t="s">
         <v>299</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="H10" s="14" t="s">
         <v>300</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="I10" s="14" t="s">
         <v>301</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>302</v>
       </c>
       <c r="K10" s="9" t="s">
         <v>105</v>
@@ -2052,40 +2065,40 @@
     </row>
     <row r="11" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2523,18 +2536,18 @@
   <sheetData>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="6" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="6" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2557,37 +2570,37 @@
     </row>
     <row r="8" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="G8" s="13" t="s">
         <v>320</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="G8" s="14" t="s">
         <v>321</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="H8" s="14" t="s">
         <v>322</v>
       </c>
+      <c r="I8" s="14" t="s">
+        <v>323</v>
+      </c>
       <c r="J8" s="9" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="L8" s="9" t="s">
         <v>105</v>
@@ -2607,53 +2620,53 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="9" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="L9" s="9"/>
       <c r="M9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3117,7 +3130,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>105</v>
@@ -3128,13 +3141,13 @@
     </row>
     <row r="4" customFormat="false" ht="100.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3317,7 +3330,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>105</v>
@@ -3328,13 +3341,13 @@
     </row>
     <row r="4" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4750,10 +4763,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A7:J37"/>
+  <dimension ref="A7:K37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4765,49 +4778,53 @@
       <c r="A7" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="3"/>
+      <c r="H7" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9"/>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="J8" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="K8" s="3" t="s">
         <v>104</v>
       </c>
     </row>
@@ -4841,6 +4858,9 @@
       </c>
       <c r="J9" s="5" t="s">
         <v>167</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4854,6 +4874,7 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11"/>
@@ -4866,6 +4887,7 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11"/>
@@ -4878,6 +4900,7 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11"/>
@@ -4890,6 +4913,7 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11"/>
@@ -4902,6 +4926,7 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11"/>
@@ -4914,6 +4939,7 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11"/>
@@ -4926,6 +4952,7 @@
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11"/>
@@ -4938,6 +4965,7 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11"/>
@@ -4950,6 +4978,7 @@
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11"/>
@@ -4962,6 +4991,7 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="11"/>
@@ -4974,6 +5004,7 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11"/>
@@ -4986,6 +5017,7 @@
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11"/>
@@ -4998,6 +5030,7 @@
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11"/>
@@ -5010,6 +5043,7 @@
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="11"/>
@@ -5022,6 +5056,7 @@
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11"/>
@@ -5034,6 +5069,7 @@
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="11"/>
@@ -5046,6 +5082,7 @@
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="11"/>
@@ -5058,6 +5095,7 @@
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11"/>
@@ -5070,6 +5108,7 @@
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="11"/>
@@ -5082,6 +5121,7 @@
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="11"/>
@@ -5094,6 +5134,7 @@
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="11"/>
@@ -5106,6 +5147,7 @@
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="11"/>
@@ -5118,6 +5160,7 @@
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="11"/>
@@ -5130,6 +5173,7 @@
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="11"/>
@@ -5142,6 +5186,7 @@
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="11"/>
@@ -5154,6 +5199,7 @@
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="11"/>
@@ -5166,6 +5212,7 @@
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="11"/>
@@ -5178,12 +5225,13 @@
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:K7"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -5223,22 +5271,22 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="6" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="6" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5252,15 +5300,15 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3" t="s">
@@ -5271,34 +5319,34 @@
     </row>
     <row r="8" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="C8" s="13" t="s">
         <v>177</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>178</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>69</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>178</v>
-      </c>
       <c r="H8" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="K8" s="9" t="s">
         <v>105</v>
@@ -5309,40 +5357,40 @@
     </row>
     <row r="9" customFormat="false" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5784,35 +5832,35 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="6" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="6" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="6" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="6" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5820,14 +5868,14 @@
         <v>155</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -5840,7 +5888,7 @@
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="M9" s="3"/>
       <c r="N9" s="3" t="s">
@@ -5851,43 +5899,43 @@
     </row>
     <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="B10" s="13" t="s">
         <v>177</v>
       </c>
+      <c r="B10" s="14" t="s">
+        <v>178</v>
+      </c>
       <c r="C10" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="J10" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="K10" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>203</v>
-      </c>
       <c r="L10" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="N10" s="9" t="s">
         <v>105</v>
@@ -5898,49 +5946,49 @@
     </row>
     <row r="11" customFormat="false" ht="158.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="N11" s="11" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6467,77 +6515,77 @@
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="6" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="6" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="6" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="6" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="6" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="6" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="6" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="6" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="6" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6545,13 +6593,13 @@
         <v>155</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6559,7 +6607,7 @@
       <c r="B16" s="9"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -6568,12 +6616,12 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="O16" s="3"/>
       <c r="P16" s="3" t="s">
@@ -6584,49 +6632,49 @@
     </row>
     <row r="17" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="C17" s="13" t="s">
         <v>177</v>
       </c>
+      <c r="C17" s="14" t="s">
+        <v>178</v>
+      </c>
       <c r="D17" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="L17" s="13" t="s">
         <v>249</v>
       </c>
+      <c r="L17" s="14" t="s">
+        <v>250</v>
+      </c>
       <c r="M17" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="N17" s="13" t="s">
         <v>251</v>
       </c>
+      <c r="N17" s="14" t="s">
+        <v>252</v>
+      </c>
       <c r="O17" s="3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="P17" s="9" t="s">
         <v>105</v>
@@ -6637,55 +6685,55 @@
     </row>
     <row r="18" customFormat="false" ht="172.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M18" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O18" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="P18" s="11" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="Q18" s="5" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7261,42 +7309,42 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="6" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="6" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="6" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="6" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="6" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="6" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="6" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7316,13 +7364,13 @@
     </row>
     <row r="12" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="B12" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>278</v>
+      <c r="B12" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>279</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>105</v>
@@ -7333,19 +7381,19 @@
     </row>
     <row r="13" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
data-model: Project, add location lat/lng
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/project-public.xlsx
+++ b/indigo/spreadsheetform_guides/project-public.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="306">
   <si>
     <t xml:space="preserve">Indigo Project ID</t>
   </si>
@@ -382,6 +382,9 @@
     <t xml:space="preserve">Location</t>
   </si>
   <si>
+    <t xml:space="preserve">Lat/Lng</t>
+  </si>
+  <si>
     <t xml:space="preserve">Adminstrative geography</t>
   </si>
   <si>
@@ -391,6 +394,12 @@
     <t xml:space="preserve">Postcode</t>
   </si>
   <si>
+    <t xml:space="preserve">Lat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lng</t>
+  </si>
+  <si>
     <t xml:space="preserve">Code Type</t>
   </si>
   <si>
@@ -407,6 +416,12 @@
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:delivery_locations:location_country/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:delivery_locations:lat_lng/lat/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:delivery_locations:lat_lng/lng/value</t>
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:delivery_locations:adminstrative_geography_name/value</t>
@@ -1162,6 +1177,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1174,15 +1197,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1856,34 +1871,34 @@
     </row>
     <row r="3" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>249</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>250</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>251</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>252</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>253</v>
+        <v>174</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>257</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>258</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>255</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>256</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>257</v>
+        <v>259</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>262</v>
       </c>
       <c r="K3" s="8" t="s">
         <v>105</v>
@@ -1894,40 +1909,40 @@
     </row>
     <row r="4" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2364,7 +2379,7 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14"/>
+      <c r="A2" s="8"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -2382,38 +2397,38 @@
       <c r="N2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
-        <v>270</v>
+      <c r="A3" s="16" t="s">
+        <v>275</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>273</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>275</v>
+        <v>277</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>280</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="L3" s="8" t="s">
         <v>105</v>
@@ -2423,7 +2438,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -2433,53 +2448,53 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="8" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="L4" s="8"/>
       <c r="M4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="72.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="16" t="s">
-        <v>280</v>
+      <c r="A5" s="10" t="s">
+        <v>285</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2943,7 +2958,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>105</v>
@@ -2954,13 +2969,13 @@
     </row>
     <row r="4" customFormat="false" ht="100.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3143,7 +3158,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>105</v>
@@ -3154,13 +3169,13 @@
     </row>
     <row r="4" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3718,10 +3733,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:J32"/>
+  <dimension ref="A2:L32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3730,12 +3745,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="39.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.87"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="27.78"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="39.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.87"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="27.78"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3745,73 +3762,89 @@
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3" t="s">
+      <c r="F2" s="11"/>
+      <c r="G2" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>100</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="129.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="129.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>129</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>128</v>
+        <v>130</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>129</v>
+        <v>132</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3822,8 +3855,10 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="10"/>
+      <c r="H5" s="5"/>
       <c r="I5" s="5"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10"/>
@@ -3833,8 +3868,10 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="10"/>
+      <c r="H6" s="5"/>
       <c r="I6" s="5"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10"/>
@@ -3844,8 +3881,10 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="10"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="5"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10"/>
@@ -3855,8 +3894,10 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="10"/>
+      <c r="H8" s="5"/>
       <c r="I8" s="5"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10"/>
@@ -3866,8 +3907,10 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="10"/>
+      <c r="H9" s="5"/>
       <c r="I9" s="5"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10"/>
@@ -3877,8 +3920,10 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="10"/>
+      <c r="H10" s="5"/>
       <c r="I10" s="5"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10"/>
@@ -3888,8 +3933,10 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="10"/>
+      <c r="H11" s="5"/>
       <c r="I11" s="5"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10"/>
@@ -3899,8 +3946,10 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="10"/>
+      <c r="H12" s="5"/>
       <c r="I12" s="5"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10"/>
@@ -3910,8 +3959,10 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="10"/>
+      <c r="H13" s="5"/>
       <c r="I13" s="5"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10"/>
@@ -3921,8 +3972,10 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="10"/>
+      <c r="H14" s="5"/>
       <c r="I14" s="5"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10"/>
@@ -3932,8 +3985,10 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="10"/>
+      <c r="H15" s="5"/>
       <c r="I15" s="5"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10"/>
@@ -3943,8 +3998,10 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="10"/>
+      <c r="H16" s="5"/>
       <c r="I16" s="5"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10"/>
@@ -3954,8 +4011,10 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="10"/>
+      <c r="H17" s="5"/>
       <c r="I17" s="5"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10"/>
@@ -3965,8 +4024,10 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
-      <c r="H18" s="10"/>
+      <c r="H18" s="5"/>
       <c r="I18" s="5"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
@@ -3976,8 +4037,10 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="10"/>
+      <c r="H19" s="5"/>
       <c r="I19" s="5"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
@@ -3987,8 +4050,10 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="10"/>
+      <c r="H20" s="5"/>
       <c r="I20" s="5"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
@@ -3998,8 +4063,10 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
-      <c r="H21" s="10"/>
+      <c r="H21" s="5"/>
       <c r="I21" s="5"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
@@ -4009,8 +4076,10 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
-      <c r="H22" s="10"/>
+      <c r="H22" s="5"/>
       <c r="I22" s="5"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
@@ -4020,8 +4089,10 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="10"/>
+      <c r="H23" s="5"/>
       <c r="I23" s="5"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10"/>
@@ -4031,8 +4102,10 @@
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="10"/>
+      <c r="H24" s="5"/>
       <c r="I24" s="5"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
@@ -4042,8 +4115,10 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="10"/>
+      <c r="H25" s="5"/>
       <c r="I25" s="5"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
@@ -4053,8 +4128,10 @@
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
-      <c r="H26" s="10"/>
+      <c r="H26" s="5"/>
       <c r="I26" s="5"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
@@ -4064,8 +4141,10 @@
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
-      <c r="H27" s="10"/>
+      <c r="H27" s="5"/>
       <c r="I27" s="5"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
@@ -4075,8 +4154,10 @@
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
-      <c r="H28" s="10"/>
+      <c r="H28" s="5"/>
       <c r="I28" s="5"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
@@ -4086,8 +4167,10 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
-      <c r="H29" s="10"/>
+      <c r="H29" s="5"/>
       <c r="I29" s="5"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="10"/>
@@ -4097,8 +4180,10 @@
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
-      <c r="H30" s="10"/>
+      <c r="H30" s="5"/>
       <c r="I30" s="5"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10"/>
@@ -4108,8 +4193,10 @@
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
-      <c r="H31" s="10"/>
+      <c r="H31" s="5"/>
       <c r="I31" s="5"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="10"/>
@@ -4119,14 +4206,17 @@
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
-      <c r="H32" s="10"/>
+      <c r="H32" s="5"/>
       <c r="I32" s="5"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -4169,25 +4259,25 @@
         <v>100</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4204,36 +4294,36 @@
       <c r="I3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
-        <v>137</v>
+      <c r="A4" s="13" t="s">
+        <v>142</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -4244,7 +4334,7 @@
       <c r="I5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -4255,7 +4345,7 @@
       <c r="I6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -4266,7 +4356,7 @@
       <c r="I7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -4277,7 +4367,7 @@
       <c r="I8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -4288,7 +4378,7 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -4299,7 +4389,7 @@
       <c r="I10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -4310,7 +4400,7 @@
       <c r="I11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -4321,7 +4411,7 @@
       <c r="I12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -4332,7 +4422,7 @@
       <c r="I13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -4343,7 +4433,7 @@
       <c r="I14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -4354,7 +4444,7 @@
       <c r="I15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -4365,7 +4455,7 @@
       <c r="I16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -4376,7 +4466,7 @@
       <c r="I17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -4387,7 +4477,7 @@
       <c r="I18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -4398,7 +4488,7 @@
       <c r="I19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="11"/>
+      <c r="A20" s="13"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -4409,7 +4499,7 @@
       <c r="I20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="11"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -4420,7 +4510,7 @@
       <c r="I21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="11"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -4431,7 +4521,7 @@
       <c r="I22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="11"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -4442,7 +4532,7 @@
       <c r="I23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="11"/>
+      <c r="A24" s="13"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -4453,7 +4543,7 @@
       <c r="I24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="11"/>
+      <c r="A25" s="13"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -4464,7 +4554,7 @@
       <c r="I25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="11"/>
+      <c r="A26" s="13"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -4475,7 +4565,7 @@
       <c r="I26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="11"/>
+      <c r="A27" s="13"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -4486,7 +4576,7 @@
       <c r="I27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="11"/>
+      <c r="A28" s="13"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -4497,7 +4587,7 @@
       <c r="I28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="11"/>
+      <c r="A29" s="13"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -4508,7 +4598,7 @@
       <c r="I29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="11"/>
+      <c r="A30" s="13"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -4519,7 +4609,7 @@
       <c r="I30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="11"/>
+      <c r="A31" s="13"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -4530,7 +4620,7 @@
       <c r="I31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="11"/>
+      <c r="A32" s="13"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -4571,18 +4661,18 @@
       <c r="A5" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B5" s="12"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="3" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -4590,32 +4680,32 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8"/>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="14" t="s">
         <v>100</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>100</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>104</v>
@@ -4623,37 +4713,37 @@
     </row>
     <row r="7" customFormat="false" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5068,15 +5158,15 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3" t="s">
@@ -5087,34 +5177,34 @@
     </row>
     <row r="3" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>171</v>
+        <v>175</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>176</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>69</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="K3" s="8" t="s">
         <v>105</v>
@@ -5125,40 +5215,40 @@
     </row>
     <row r="4" customFormat="false" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5602,7 +5692,7 @@
       <c r="A2" s="8"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -5615,7 +5705,7 @@
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="M2" s="3"/>
       <c r="N2" s="3" t="s">
@@ -5626,43 +5716,43 @@
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>171</v>
+        <v>175</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>176</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>190</v>
-      </c>
       <c r="J3" s="3" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>105</v>
@@ -5673,49 +5763,49 @@
     </row>
     <row r="4" customFormat="false" ht="158.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="N4" s="10" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6243,7 +6333,7 @@
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C1" s="6"/>
       <c r="K1" s="0" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="L1" s="6"/>
       <c r="N1" s="6"/>
@@ -6253,7 +6343,7 @@
       <c r="B2" s="8"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -6262,12 +6352,12 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="O2" s="3"/>
       <c r="P2" s="3" t="s">
@@ -6278,49 +6368,49 @@
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>171</v>
+        <v>175</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>176</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>222</v>
+        <v>226</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>227</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>224</v>
+        <v>228</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>229</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="P3" s="8" t="s">
         <v>105</v>
@@ -6331,55 +6421,55 @@
     </row>
     <row r="4" customFormat="false" ht="172.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6965,13 +7055,13 @@
     </row>
     <row r="3" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>243</v>
+        <v>175</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>248</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>105</v>
@@ -6982,19 +7072,19 @@
     </row>
     <row r="4" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>